<commit_message>
excel tablosuna yapılan ekleme değiştirme silme işlemleri database ile senkron şekilde gerceklesiyor
</commit_message>
<xml_diff>
--- a/WebApplication1/Forms/03_EgzozValf.xlsx
+++ b/WebApplication1/Forms/03_EgzozValf.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\serdar.dal\Desktop\Forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\serdar.dal\source\repos\WebApplication1\WebApplication1\Forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="4755" windowWidth="28560" windowHeight="10140"/>
+    <workbookView xWindow="120" yWindow="4752" windowWidth="28560" windowHeight="10140"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -405,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -529,6 +529,9 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1577,51 +1580,51 @@
   <dimension ref="A1:P76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56:F58"/>
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="79" t="s">
+    <row r="1" spans="1:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="81"/>
-    </row>
-    <row r="2" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="82"/>
+    </row>
+    <row r="2" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="75" t="s">
+      <c r="B2" s="74"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="76"/>
-      <c r="F2" s="90" t="s">
+      <c r="E2" s="77"/>
+      <c r="F2" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="91"/>
+      <c r="G2" s="92"/>
       <c r="H2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="85"/>
-      <c r="J2" s="86"/>
-    </row>
-    <row r="3" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I2" s="86"/>
+      <c r="J2" s="87"/>
+    </row>
+    <row r="3" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
         <v>34</v>
       </c>
@@ -1630,53 +1633,53 @@
         <v>35</v>
       </c>
       <c r="D3" s="45"/>
-      <c r="E3" s="71" t="s">
+      <c r="E3" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="72"/>
+      <c r="F3" s="73"/>
       <c r="G3" s="46"/>
       <c r="H3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="73"/>
-      <c r="J3" s="74"/>
-    </row>
-    <row r="4" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="87" t="s">
+      <c r="I3" s="74"/>
+      <c r="J3" s="75"/>
+    </row>
+    <row r="4" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="88"/>
-      <c r="C4" s="88"/>
-      <c r="D4" s="89"/>
+      <c r="B4" s="89"/>
+      <c r="C4" s="89"/>
+      <c r="D4" s="90"/>
       <c r="E4" s="47"/>
-      <c r="F4" s="75" t="s">
+      <c r="F4" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="76"/>
+      <c r="G4" s="77"/>
       <c r="H4" s="47"/>
       <c r="I4" s="23" t="s">
         <v>5</v>
       </c>
       <c r="J4" s="47"/>
     </row>
-    <row r="5" spans="1:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="63" t="s">
+    <row r="5" spans="1:16" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="64"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="92" t="s">
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="93"/>
-      <c r="I5" s="93"/>
-      <c r="J5" s="94"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="94"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="95"/>
       <c r="K5" s="44"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="36"/>
       <c r="B6" s="37"/>
       <c r="C6" s="37"/>
@@ -1688,7 +1691,7 @@
       <c r="I6" s="41"/>
       <c r="J6" s="42"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1700,7 +1703,7 @@
       <c r="I7" s="4"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1713,7 +1716,7 @@
       <c r="J8" s="5"/>
       <c r="P8" s="16"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1726,7 +1729,7 @@
       <c r="J9" s="5"/>
       <c r="P9" s="16"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1738,7 +1741,7 @@
       <c r="I10" s="4"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1750,7 +1753,7 @@
       <c r="I11" s="4"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1762,7 +1765,7 @@
       <c r="I12" s="4"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1774,7 +1777,7 @@
       <c r="I13" s="4"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1786,7 +1789,7 @@
       <c r="I14" s="4"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1799,7 +1802,7 @@
       <c r="J15" s="5"/>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1811,7 +1814,7 @@
       <c r="I16" s="4"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1823,7 +1826,7 @@
       <c r="I17" s="4"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -1835,12 +1838,12 @@
       <c r="I18" s="4"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="73"/>
-      <c r="C19" s="74"/>
+      <c r="B19" s="74"/>
+      <c r="C19" s="75"/>
       <c r="D19" s="28" t="s">
         <v>31</v>
       </c>
@@ -1851,7 +1854,7 @@
       <c r="I19" s="4"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="29" t="s">
         <v>30</v>
       </c>
@@ -1865,11 +1868,11 @@
       <c r="I20" s="4"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="71" t="s">
+    <row r="21" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="72"/>
+      <c r="B21" s="73"/>
       <c r="C21" s="48"/>
       <c r="D21" s="33" t="s">
         <v>33</v>
@@ -1881,45 +1884,45 @@
       <c r="I21" s="7"/>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="71" t="s">
+    <row r="22" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="72"/>
+      <c r="B22" s="73"/>
       <c r="C22" s="48"/>
       <c r="D22" s="49"/>
-      <c r="E22" s="75" t="s">
+      <c r="E22" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="76"/>
+      <c r="F22" s="77"/>
       <c r="G22" s="45"/>
       <c r="H22" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I22" s="77"/>
-      <c r="J22" s="78"/>
-    </row>
-    <row r="23" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="82" t="s">
+      <c r="I22" s="78"/>
+      <c r="J22" s="79"/>
+    </row>
+    <row r="23" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="83"/>
-      <c r="C23" s="83"/>
-      <c r="D23" s="83"/>
-      <c r="E23" s="83"/>
-      <c r="F23" s="83"/>
-      <c r="G23" s="83"/>
-      <c r="H23" s="83"/>
-      <c r="I23" s="83"/>
-      <c r="J23" s="84"/>
+      <c r="B23" s="84"/>
+      <c r="C23" s="84"/>
+      <c r="D23" s="84"/>
+      <c r="E23" s="84"/>
+      <c r="F23" s="84"/>
+      <c r="G23" s="84"/>
+      <c r="H23" s="84"/>
+      <c r="I23" s="84"/>
+      <c r="J23" s="85"/>
       <c r="L23" s="31"/>
     </row>
-    <row r="24" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="73"/>
-      <c r="C24" s="74"/>
+      <c r="B24" s="74"/>
+      <c r="C24" s="75"/>
       <c r="D24" s="34" t="s">
         <v>32</v>
       </c>
@@ -1934,7 +1937,7 @@
       </c>
       <c r="J24" s="49"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="4"/>
       <c r="C25" s="5"/>
@@ -1943,36 +1946,36 @@
       <c r="F25" s="21"/>
       <c r="G25" s="10"/>
       <c r="H25" s="5"/>
-      <c r="I25" s="68" t="s">
+      <c r="I25" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="J25" s="61"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J25" s="62"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
       <c r="C26" s="5"/>
-      <c r="D26" s="66"/>
+      <c r="D26" s="67"/>
       <c r="E26" s="4"/>
       <c r="F26" s="21"/>
       <c r="G26" s="10"/>
       <c r="H26" s="5"/>
-      <c r="I26" s="68"/>
-      <c r="J26" s="61"/>
-    </row>
-    <row r="27" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I26" s="69"/>
+      <c r="J26" s="62"/>
+    </row>
+    <row r="27" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="4"/>
       <c r="C27" s="5"/>
-      <c r="D27" s="66"/>
+      <c r="D27" s="67"/>
       <c r="E27" s="4"/>
       <c r="F27" s="21"/>
       <c r="G27" s="10"/>
       <c r="H27" s="5"/>
-      <c r="I27" s="69"/>
-      <c r="J27" s="62"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I27" s="70"/>
+      <c r="J27" s="63"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="4"/>
       <c r="C28" s="5"/>
@@ -1981,12 +1984,12 @@
       <c r="F28" s="21"/>
       <c r="G28" s="10"/>
       <c r="H28" s="5"/>
-      <c r="I28" s="67" t="s">
+      <c r="I28" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="J28" s="61"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J28" s="62"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="4"/>
       <c r="C29" s="5"/>
@@ -1995,10 +1998,10 @@
       <c r="F29" s="21"/>
       <c r="G29" s="10"/>
       <c r="H29" s="5"/>
-      <c r="I29" s="68"/>
-      <c r="J29" s="61"/>
-    </row>
-    <row r="30" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I29" s="69"/>
+      <c r="J29" s="62"/>
+    </row>
+    <row r="30" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
       <c r="C30" s="5"/>
@@ -2007,10 +2010,10 @@
       <c r="F30" s="21"/>
       <c r="G30" s="10"/>
       <c r="H30" s="5"/>
-      <c r="I30" s="69"/>
-      <c r="J30" s="62"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I30" s="70"/>
+      <c r="J30" s="63"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="4"/>
       <c r="C31" s="5"/>
@@ -2019,36 +2022,36 @@
       <c r="F31" s="21"/>
       <c r="G31" s="10"/>
       <c r="H31" s="5"/>
-      <c r="I31" s="67" t="s">
+      <c r="I31" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="J31" s="61"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J31" s="62"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="4"/>
       <c r="C32" s="5"/>
-      <c r="D32" s="66"/>
+      <c r="D32" s="67"/>
       <c r="E32" s="4"/>
       <c r="F32" s="21"/>
       <c r="G32" s="10"/>
       <c r="H32" s="5"/>
-      <c r="I32" s="68"/>
-      <c r="J32" s="61"/>
-    </row>
-    <row r="33" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I32" s="69"/>
+      <c r="J32" s="62"/>
+    </row>
+    <row r="33" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
-      <c r="D33" s="66"/>
+      <c r="D33" s="67"/>
       <c r="E33" s="4"/>
       <c r="F33" s="21"/>
       <c r="G33" s="10"/>
       <c r="H33" s="5"/>
-      <c r="I33" s="69"/>
-      <c r="J33" s="62"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I33" s="70"/>
+      <c r="J33" s="63"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="4"/>
       <c r="C34" s="5"/>
@@ -2057,12 +2060,12 @@
       <c r="F34" s="21"/>
       <c r="G34" s="10"/>
       <c r="H34" s="5"/>
-      <c r="I34" s="67" t="s">
+      <c r="I34" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="J34" s="61"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J34" s="62"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="4"/>
       <c r="C35" s="5"/>
@@ -2071,10 +2074,10 @@
       <c r="F35" s="21"/>
       <c r="G35" s="10"/>
       <c r="H35" s="5"/>
-      <c r="I35" s="68"/>
-      <c r="J35" s="61"/>
-    </row>
-    <row r="36" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I35" s="69"/>
+      <c r="J35" s="62"/>
+    </row>
+    <row r="36" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="4"/>
       <c r="C36" s="5"/>
@@ -2083,10 +2086,10 @@
       <c r="F36" s="21"/>
       <c r="G36" s="10"/>
       <c r="H36" s="5"/>
-      <c r="I36" s="69"/>
-      <c r="J36" s="62"/>
-    </row>
-    <row r="37" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I36" s="70"/>
+      <c r="J36" s="63"/>
+    </row>
+    <row r="37" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="4"/>
       <c r="C37" s="5"/>
@@ -2095,12 +2098,12 @@
       <c r="F37" s="3"/>
       <c r="G37" s="4"/>
       <c r="H37" s="5"/>
-      <c r="I37" s="67" t="s">
+      <c r="I37" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="J37" s="61"/>
-    </row>
-    <row r="38" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J37" s="62"/>
+    </row>
+    <row r="38" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="15"/>
       <c r="B38" s="14"/>
       <c r="C38" s="13"/>
@@ -2111,15 +2114,15 @@
       <c r="F38" s="19"/>
       <c r="G38" s="10"/>
       <c r="H38" s="18"/>
-      <c r="I38" s="68"/>
-      <c r="J38" s="61"/>
-    </row>
-    <row r="39" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I38" s="69"/>
+      <c r="J38" s="62"/>
+    </row>
+    <row r="39" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="59"/>
-      <c r="C39" s="60"/>
+      <c r="B39" s="60"/>
+      <c r="C39" s="61"/>
       <c r="D39" s="26" t="s">
         <v>24</v>
       </c>
@@ -2127,24 +2130,24 @@
       <c r="F39" s="15"/>
       <c r="G39" s="22"/>
       <c r="H39" s="20"/>
-      <c r="I39" s="69"/>
-      <c r="J39" s="62"/>
-    </row>
-    <row r="40" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="63" t="s">
+      <c r="I39" s="70"/>
+      <c r="J39" s="63"/>
+    </row>
+    <row r="40" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="B40" s="64"/>
-      <c r="C40" s="64"/>
-      <c r="D40" s="64"/>
-      <c r="E40" s="64"/>
-      <c r="F40" s="64"/>
-      <c r="G40" s="64"/>
-      <c r="H40" s="64"/>
-      <c r="I40" s="64"/>
-      <c r="J40" s="65"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B40" s="65"/>
+      <c r="C40" s="65"/>
+      <c r="D40" s="65"/>
+      <c r="E40" s="65"/>
+      <c r="F40" s="65"/>
+      <c r="G40" s="65"/>
+      <c r="H40" s="65"/>
+      <c r="I40" s="65"/>
+      <c r="J40" s="66"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -2156,7 +2159,7 @@
       <c r="I41" s="4"/>
       <c r="J41" s="5"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -2168,7 +2171,7 @@
       <c r="I42" s="4"/>
       <c r="J42" s="5"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -2180,7 +2183,7 @@
       <c r="I43" s="4"/>
       <c r="J43" s="5"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -2192,7 +2195,7 @@
       <c r="I44" s="4"/>
       <c r="J44" s="5"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -2204,7 +2207,7 @@
       <c r="I45" s="4"/>
       <c r="J45" s="5"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -2216,7 +2219,7 @@
       <c r="I46" s="4"/>
       <c r="J46" s="5"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -2228,7 +2231,7 @@
       <c r="I47" s="4"/>
       <c r="J47" s="5"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -2240,7 +2243,7 @@
       <c r="I48" s="4"/>
       <c r="J48" s="5"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -2252,7 +2255,7 @@
       <c r="I49" s="4"/>
       <c r="J49" s="5"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -2264,7 +2267,7 @@
       <c r="I50" s="4"/>
       <c r="J50" s="5"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -2276,7 +2279,7 @@
       <c r="I51" s="4"/>
       <c r="J51" s="5"/>
     </row>
-    <row r="52" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="6"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
@@ -2288,121 +2291,121 @@
       <c r="I52" s="4"/>
       <c r="J52" s="5"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="2"/>
-      <c r="E53" s="67" t="s">
+      <c r="E53" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="F53" s="70"/>
+      <c r="F53" s="71"/>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
       <c r="J53" s="5"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="5"/>
-      <c r="E54" s="68"/>
-      <c r="F54" s="61"/>
+      <c r="E54" s="69"/>
+      <c r="F54" s="62"/>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
       <c r="J54" s="5"/>
     </row>
-    <row r="55" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="5"/>
-      <c r="E55" s="69"/>
-      <c r="F55" s="62"/>
+      <c r="E55" s="70"/>
+      <c r="F55" s="63"/>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
       <c r="J55" s="5"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="5"/>
-      <c r="E56" s="67" t="s">
+      <c r="E56" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="F56" s="70"/>
+      <c r="F56" s="71"/>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
       <c r="J56" s="5"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="5"/>
-      <c r="E57" s="68"/>
-      <c r="F57" s="61"/>
+      <c r="E57" s="69"/>
+      <c r="F57" s="62"/>
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
       <c r="J57" s="5"/>
     </row>
-    <row r="58" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="5"/>
-      <c r="E58" s="69"/>
-      <c r="F58" s="62"/>
+      <c r="E58" s="70"/>
+      <c r="F58" s="63"/>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
       <c r="J58" s="5"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="5"/>
-      <c r="E59" s="67" t="s">
+      <c r="E59" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="F59" s="70"/>
+      <c r="F59" s="71"/>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
       <c r="J59" s="5"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="5"/>
-      <c r="E60" s="68"/>
-      <c r="F60" s="61"/>
+      <c r="E60" s="69"/>
+      <c r="F60" s="62"/>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
       <c r="J60" s="5"/>
     </row>
-    <row r="61" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="5"/>
-      <c r="E61" s="69"/>
-      <c r="F61" s="62"/>
+      <c r="E61" s="70"/>
+      <c r="F61" s="63"/>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
       <c r="J61" s="5"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -2414,7 +2417,7 @@
       <c r="I62" s="4"/>
       <c r="J62" s="5"/>
     </row>
-    <row r="63" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="6"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
@@ -2423,10 +2426,10 @@
       <c r="F63" s="56"/>
       <c r="G63" s="7"/>
       <c r="H63" s="7"/>
-      <c r="I63" s="57"/>
-      <c r="J63" s="58"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I63" s="58"/>
+      <c r="J63" s="59"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -2439,7 +2442,7 @@
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
@@ -2451,7 +2454,7 @@
       <c r="I65" s="4"/>
       <c r="J65" s="4"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
@@ -2463,25 +2466,16 @@
       <c r="I66" s="4"/>
       <c r="J66" s="4"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L75" s="4"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L76" s="4"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <dataConsolidate/>
   <mergeCells count="39">
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="J25:J27"/>
-    <mergeCell ref="I31:I33"/>
-    <mergeCell ref="I34:I36"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="J28:J30"/>
-    <mergeCell ref="J31:J33"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A23:J23"/>
     <mergeCell ref="I2:J2"/>
@@ -2492,8 +2486,10 @@
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E5:J5"/>
     <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F56:F58"/>
-    <mergeCell ref="F59:F61"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="B19:C19"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="J34:J36"/>
     <mergeCell ref="B24:C24"/>
@@ -2502,6 +2498,11 @@
     <mergeCell ref="D26:D27"/>
     <mergeCell ref="I25:I27"/>
     <mergeCell ref="I28:I30"/>
+    <mergeCell ref="J25:J27"/>
+    <mergeCell ref="I31:I33"/>
+    <mergeCell ref="I34:I36"/>
+    <mergeCell ref="J28:J30"/>
+    <mergeCell ref="J31:J33"/>
     <mergeCell ref="I63:J63"/>
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="J37:J39"/>
@@ -2512,6 +2513,8 @@
     <mergeCell ref="E56:E58"/>
     <mergeCell ref="E59:E61"/>
     <mergeCell ref="F53:F55"/>
+    <mergeCell ref="F56:F58"/>
+    <mergeCell ref="F59:F61"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2524,26 +2527,103 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="57"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="57"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="57"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="57"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+    </row>
+  </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="57"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="57"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="57"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="57"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+    </row>
+  </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>

<commit_message>
kayıt etme ve güncelleme işlemleri temp file üzerinden yapılıyor
</commit_message>
<xml_diff>
--- a/WebApplication1/Forms/03_EgzozValf.xlsx
+++ b/WebApplication1/Forms/03_EgzozValf.xlsx
@@ -534,19 +534,84 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -556,108 +621,43 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1224,69 +1224,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1098" name="Rectangle 9"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="6610350"/>
-          <a:ext cx="6657975" cy="209550"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:effectLst>
-                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="808080"/>
-                </a:outerShdw>
-              </a:effectLst>
-            </a14:hiddenEffects>
-          </a:ext>
-          <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
-            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="1"/>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1579,8 +1516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1591,38 +1528,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
-      <c r="J1" s="82"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="60"/>
     </row>
     <row r="2" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="76" t="s">
+      <c r="B2" s="66"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="77"/>
-      <c r="F2" s="91" t="s">
+      <c r="E2" s="69"/>
+      <c r="F2" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="92"/>
+      <c r="G2" s="74"/>
       <c r="H2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="86"/>
-      <c r="J2" s="87"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="65"/>
     </row>
     <row r="3" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
@@ -1633,29 +1570,29 @@
         <v>35</v>
       </c>
       <c r="D3" s="45"/>
-      <c r="E3" s="72" t="s">
+      <c r="E3" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="73"/>
+      <c r="F3" s="76"/>
       <c r="G3" s="46"/>
       <c r="H3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="74"/>
-      <c r="J3" s="75"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="67"/>
     </row>
     <row r="4" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="88" t="s">
+      <c r="A4" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="89"/>
-      <c r="C4" s="89"/>
-      <c r="D4" s="90"/>
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="72"/>
       <c r="E4" s="47"/>
-      <c r="F4" s="76" t="s">
+      <c r="F4" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="77"/>
+      <c r="G4" s="69"/>
       <c r="H4" s="47"/>
       <c r="I4" s="23" t="s">
         <v>5</v>
@@ -1663,20 +1600,20 @@
       <c r="J4" s="47"/>
     </row>
     <row r="5" spans="1:16" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="65"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="93" t="s">
+      <c r="B5" s="81"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="82"/>
+      <c r="E5" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="94"/>
-      <c r="G5" s="94"/>
-      <c r="H5" s="94"/>
-      <c r="I5" s="94"/>
-      <c r="J5" s="95"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="78"/>
+      <c r="I5" s="78"/>
+      <c r="J5" s="79"/>
       <c r="K5" s="44"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -1842,8 +1779,8 @@
       <c r="A19" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="74"/>
-      <c r="C19" s="75"/>
+      <c r="B19" s="66"/>
+      <c r="C19" s="67"/>
       <c r="D19" s="28" t="s">
         <v>31</v>
       </c>
@@ -1869,10 +1806,10 @@
       <c r="J20" s="5"/>
     </row>
     <row r="21" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="72" t="s">
+      <c r="A21" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="73"/>
+      <c r="B21" s="76"/>
       <c r="C21" s="48"/>
       <c r="D21" s="33" t="s">
         <v>33</v>
@@ -1885,44 +1822,44 @@
       <c r="J21" s="8"/>
     </row>
     <row r="22" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="72" t="s">
+      <c r="A22" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="73"/>
+      <c r="B22" s="76"/>
       <c r="C22" s="48"/>
       <c r="D22" s="49"/>
-      <c r="E22" s="76" t="s">
+      <c r="E22" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="77"/>
+      <c r="F22" s="69"/>
       <c r="G22" s="45"/>
       <c r="H22" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I22" s="78"/>
-      <c r="J22" s="79"/>
+      <c r="I22" s="85"/>
+      <c r="J22" s="86"/>
     </row>
     <row r="23" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="83" t="s">
+      <c r="A23" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="84"/>
-      <c r="C23" s="84"/>
-      <c r="D23" s="84"/>
-      <c r="E23" s="84"/>
-      <c r="F23" s="84"/>
-      <c r="G23" s="84"/>
-      <c r="H23" s="84"/>
-      <c r="I23" s="84"/>
-      <c r="J23" s="85"/>
+      <c r="B23" s="62"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="63"/>
       <c r="L23" s="31"/>
     </row>
     <row r="24" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="74"/>
-      <c r="C24" s="75"/>
+      <c r="B24" s="66"/>
+      <c r="C24" s="67"/>
       <c r="D24" s="34" t="s">
         <v>32</v>
       </c>
@@ -1946,34 +1883,34 @@
       <c r="F25" s="21"/>
       <c r="G25" s="10"/>
       <c r="H25" s="5"/>
-      <c r="I25" s="69" t="s">
+      <c r="I25" s="88" t="s">
         <v>14</v>
       </c>
-      <c r="J25" s="62"/>
+      <c r="J25" s="83"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
       <c r="C26" s="5"/>
-      <c r="D26" s="67"/>
+      <c r="D26" s="87"/>
       <c r="E26" s="4"/>
       <c r="F26" s="21"/>
       <c r="G26" s="10"/>
       <c r="H26" s="5"/>
-      <c r="I26" s="69"/>
-      <c r="J26" s="62"/>
+      <c r="I26" s="88"/>
+      <c r="J26" s="83"/>
     </row>
     <row r="27" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="4"/>
       <c r="C27" s="5"/>
-      <c r="D27" s="67"/>
+      <c r="D27" s="87"/>
       <c r="E27" s="4"/>
       <c r="F27" s="21"/>
       <c r="G27" s="10"/>
       <c r="H27" s="5"/>
-      <c r="I27" s="70"/>
-      <c r="J27" s="63"/>
+      <c r="I27" s="89"/>
+      <c r="J27" s="84"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
@@ -1984,10 +1921,10 @@
       <c r="F28" s="21"/>
       <c r="G28" s="10"/>
       <c r="H28" s="5"/>
-      <c r="I28" s="68" t="s">
+      <c r="I28" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="J28" s="62"/>
+      <c r="J28" s="83"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
@@ -1998,8 +1935,8 @@
       <c r="F29" s="21"/>
       <c r="G29" s="10"/>
       <c r="H29" s="5"/>
-      <c r="I29" s="69"/>
-      <c r="J29" s="62"/>
+      <c r="I29" s="88"/>
+      <c r="J29" s="83"/>
     </row>
     <row r="30" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
@@ -2010,8 +1947,8 @@
       <c r="F30" s="21"/>
       <c r="G30" s="10"/>
       <c r="H30" s="5"/>
-      <c r="I30" s="70"/>
-      <c r="J30" s="63"/>
+      <c r="I30" s="89"/>
+      <c r="J30" s="84"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
@@ -2022,34 +1959,34 @@
       <c r="F31" s="21"/>
       <c r="G31" s="10"/>
       <c r="H31" s="5"/>
-      <c r="I31" s="68" t="s">
+      <c r="I31" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="J31" s="62"/>
+      <c r="J31" s="83"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="4"/>
       <c r="C32" s="5"/>
-      <c r="D32" s="67"/>
+      <c r="D32" s="87"/>
       <c r="E32" s="4"/>
       <c r="F32" s="21"/>
       <c r="G32" s="10"/>
       <c r="H32" s="5"/>
-      <c r="I32" s="69"/>
-      <c r="J32" s="62"/>
+      <c r="I32" s="88"/>
+      <c r="J32" s="83"/>
     </row>
     <row r="33" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
-      <c r="D33" s="67"/>
+      <c r="D33" s="87"/>
       <c r="E33" s="4"/>
       <c r="F33" s="21"/>
       <c r="G33" s="10"/>
       <c r="H33" s="5"/>
-      <c r="I33" s="70"/>
-      <c r="J33" s="63"/>
+      <c r="I33" s="89"/>
+      <c r="J33" s="84"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
@@ -2060,10 +1997,10 @@
       <c r="F34" s="21"/>
       <c r="G34" s="10"/>
       <c r="H34" s="5"/>
-      <c r="I34" s="68" t="s">
+      <c r="I34" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="J34" s="62"/>
+      <c r="J34" s="83"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
@@ -2074,8 +2011,8 @@
       <c r="F35" s="21"/>
       <c r="G35" s="10"/>
       <c r="H35" s="5"/>
-      <c r="I35" s="69"/>
-      <c r="J35" s="62"/>
+      <c r="I35" s="88"/>
+      <c r="J35" s="83"/>
     </row>
     <row r="36" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
@@ -2086,8 +2023,8 @@
       <c r="F36" s="21"/>
       <c r="G36" s="10"/>
       <c r="H36" s="5"/>
-      <c r="I36" s="70"/>
-      <c r="J36" s="63"/>
+      <c r="I36" s="89"/>
+      <c r="J36" s="84"/>
     </row>
     <row r="37" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
@@ -2098,10 +2035,10 @@
       <c r="F37" s="3"/>
       <c r="G37" s="4"/>
       <c r="H37" s="5"/>
-      <c r="I37" s="68" t="s">
+      <c r="I37" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="J37" s="62"/>
+      <c r="J37" s="83"/>
     </row>
     <row r="38" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="15"/>
@@ -2114,15 +2051,15 @@
       <c r="F38" s="19"/>
       <c r="G38" s="10"/>
       <c r="H38" s="18"/>
-      <c r="I38" s="69"/>
-      <c r="J38" s="62"/>
+      <c r="I38" s="88"/>
+      <c r="J38" s="83"/>
     </row>
     <row r="39" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="60"/>
-      <c r="C39" s="61"/>
+      <c r="B39" s="93"/>
+      <c r="C39" s="94"/>
       <c r="D39" s="26" t="s">
         <v>24</v>
       </c>
@@ -2130,22 +2067,22 @@
       <c r="F39" s="15"/>
       <c r="G39" s="22"/>
       <c r="H39" s="20"/>
-      <c r="I39" s="70"/>
-      <c r="J39" s="63"/>
+      <c r="I39" s="89"/>
+      <c r="J39" s="84"/>
     </row>
     <row r="40" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="64" t="s">
+      <c r="A40" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="B40" s="65"/>
-      <c r="C40" s="65"/>
-      <c r="D40" s="65"/>
-      <c r="E40" s="65"/>
-      <c r="F40" s="65"/>
-      <c r="G40" s="65"/>
-      <c r="H40" s="65"/>
-      <c r="I40" s="65"/>
-      <c r="J40" s="66"/>
+      <c r="B40" s="81"/>
+      <c r="C40" s="81"/>
+      <c r="D40" s="81"/>
+      <c r="E40" s="81"/>
+      <c r="F40" s="81"/>
+      <c r="G40" s="81"/>
+      <c r="H40" s="81"/>
+      <c r="I40" s="81"/>
+      <c r="J40" s="82"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
@@ -2296,10 +2233,10 @@
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="2"/>
-      <c r="E53" s="68" t="s">
+      <c r="E53" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="F53" s="71"/>
+      <c r="F53" s="95"/>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
@@ -2310,8 +2247,8 @@
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="5"/>
-      <c r="E54" s="69"/>
-      <c r="F54" s="62"/>
+      <c r="E54" s="88"/>
+      <c r="F54" s="83"/>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
@@ -2322,8 +2259,8 @@
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="5"/>
-      <c r="E55" s="70"/>
-      <c r="F55" s="63"/>
+      <c r="E55" s="89"/>
+      <c r="F55" s="84"/>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
@@ -2334,10 +2271,10 @@
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="5"/>
-      <c r="E56" s="68" t="s">
+      <c r="E56" s="90" t="s">
         <v>26</v>
       </c>
-      <c r="F56" s="71"/>
+      <c r="F56" s="95"/>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
@@ -2348,8 +2285,8 @@
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="5"/>
-      <c r="E57" s="69"/>
-      <c r="F57" s="62"/>
+      <c r="E57" s="88"/>
+      <c r="F57" s="83"/>
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
@@ -2360,8 +2297,8 @@
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="5"/>
-      <c r="E58" s="70"/>
-      <c r="F58" s="63"/>
+      <c r="E58" s="89"/>
+      <c r="F58" s="84"/>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
@@ -2372,10 +2309,10 @@
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="5"/>
-      <c r="E59" s="68" t="s">
+      <c r="E59" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="F59" s="71"/>
+      <c r="F59" s="95"/>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
@@ -2386,8 +2323,8 @@
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="5"/>
-      <c r="E60" s="69"/>
-      <c r="F60" s="62"/>
+      <c r="E60" s="88"/>
+      <c r="F60" s="83"/>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
@@ -2398,8 +2335,8 @@
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="5"/>
-      <c r="E61" s="70"/>
-      <c r="F61" s="63"/>
+      <c r="E61" s="89"/>
+      <c r="F61" s="84"/>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
@@ -2426,8 +2363,8 @@
       <c r="F63" s="56"/>
       <c r="G63" s="7"/>
       <c r="H63" s="7"/>
-      <c r="I63" s="58"/>
-      <c r="J63" s="59"/>
+      <c r="I63" s="91"/>
+      <c r="J63" s="92"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
@@ -2476,6 +2413,30 @@
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <dataConsolidate/>
   <mergeCells count="39">
+    <mergeCell ref="I63:J63"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="J37:J39"/>
+    <mergeCell ref="A40:J40"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="I37:I39"/>
+    <mergeCell ref="E53:E55"/>
+    <mergeCell ref="E56:E58"/>
+    <mergeCell ref="E59:E61"/>
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="F56:F58"/>
+    <mergeCell ref="F59:F61"/>
+    <mergeCell ref="J34:J36"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="I25:I27"/>
+    <mergeCell ref="I28:I30"/>
+    <mergeCell ref="J25:J27"/>
+    <mergeCell ref="I31:I33"/>
+    <mergeCell ref="I34:I36"/>
+    <mergeCell ref="J28:J30"/>
+    <mergeCell ref="J31:J33"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A23:J23"/>
     <mergeCell ref="I2:J2"/>
@@ -2491,30 +2452,6 @@
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="A22:B22"/>
-    <mergeCell ref="J34:J36"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="I25:I27"/>
-    <mergeCell ref="I28:I30"/>
-    <mergeCell ref="J25:J27"/>
-    <mergeCell ref="I31:I33"/>
-    <mergeCell ref="I34:I36"/>
-    <mergeCell ref="J28:J30"/>
-    <mergeCell ref="J31:J33"/>
-    <mergeCell ref="I63:J63"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="J37:J39"/>
-    <mergeCell ref="A40:J40"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="I37:I39"/>
-    <mergeCell ref="E53:E55"/>
-    <mergeCell ref="E56:E58"/>
-    <mergeCell ref="E59:E61"/>
-    <mergeCell ref="F53:F55"/>
-    <mergeCell ref="F56:F58"/>
-    <mergeCell ref="F59:F61"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
hücrelerin formatı gönderiliyor ve kayıt ederken doğruluğu kontrol ediliyor
</commit_message>
<xml_diff>
--- a/WebApplication1/Forms/03_EgzozValf.xlsx
+++ b/WebApplication1/Forms/03_EgzozValf.xlsx
@@ -405,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -492,13 +492,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -532,6 +525,88 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -556,23 +631,17 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="14" fontId="5" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -604,59 +673,12 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="2" fontId="5" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1516,8 +1538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:J40"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1528,92 +1550,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="60"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="82"/>
     </row>
     <row r="2" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="68" t="s">
+      <c r="B2" s="88"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="69"/>
-      <c r="F2" s="73" t="s">
+      <c r="E2" s="77"/>
+      <c r="F2" s="93" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="74"/>
+      <c r="G2" s="94"/>
       <c r="H2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="64"/>
-      <c r="J2" s="65"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="87"/>
     </row>
     <row r="3" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="45"/>
+      <c r="B3" s="59"/>
       <c r="C3" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="75" t="s">
+      <c r="D3" s="56"/>
+      <c r="E3" s="95" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="76"/>
-      <c r="G3" s="46"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="57"/>
       <c r="H3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="66"/>
-      <c r="J3" s="67"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="101"/>
     </row>
     <row r="4" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="68" t="s">
+      <c r="B4" s="91"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="92"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="69"/>
-      <c r="H4" s="47"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="58"/>
       <c r="I4" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="47"/>
+      <c r="J4" s="58"/>
     </row>
     <row r="5" spans="1:16" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="80" t="s">
+      <c r="A5" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="82"/>
-      <c r="E5" s="77" t="s">
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="79"/>
+      <c r="F5" s="98"/>
+      <c r="G5" s="98"/>
+      <c r="H5" s="98"/>
+      <c r="I5" s="98"/>
+      <c r="J5" s="99"/>
       <c r="K5" s="44"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -1779,8 +1801,8 @@
       <c r="A19" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="66"/>
-      <c r="C19" s="67"/>
+      <c r="B19" s="74"/>
+      <c r="C19" s="75"/>
       <c r="D19" s="28" t="s">
         <v>31</v>
       </c>
@@ -1796,8 +1818,8 @@
         <v>30</v>
       </c>
       <c r="B20" s="27"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="49"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="47"/>
       <c r="E20" s="3"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -1806,11 +1828,11 @@
       <c r="J20" s="5"/>
     </row>
     <row r="21" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="75" t="s">
+      <c r="A21" s="95" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="76"/>
-      <c r="C21" s="48"/>
+      <c r="B21" s="96"/>
+      <c r="C21" s="46"/>
       <c r="D21" s="33" t="s">
         <v>33</v>
       </c>
@@ -1822,44 +1844,44 @@
       <c r="J21" s="8"/>
     </row>
     <row r="22" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="75" t="s">
+      <c r="A22" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="76"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="68" t="s">
+      <c r="B22" s="96"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="69"/>
+      <c r="F22" s="77"/>
       <c r="G22" s="45"/>
       <c r="H22" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I22" s="85"/>
-      <c r="J22" s="86"/>
+      <c r="I22" s="78"/>
+      <c r="J22" s="79"/>
     </row>
     <row r="23" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="61" t="s">
+      <c r="A23" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="62"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="63"/>
+      <c r="B23" s="84"/>
+      <c r="C23" s="84"/>
+      <c r="D23" s="84"/>
+      <c r="E23" s="84"/>
+      <c r="F23" s="84"/>
+      <c r="G23" s="84"/>
+      <c r="H23" s="84"/>
+      <c r="I23" s="84"/>
+      <c r="J23" s="85"/>
       <c r="L23" s="31"/>
     </row>
     <row r="24" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="66"/>
-      <c r="C24" s="67"/>
+      <c r="B24" s="74"/>
+      <c r="C24" s="75"/>
       <c r="D24" s="34" t="s">
         <v>32</v>
       </c>
@@ -1868,11 +1890,11 @@
         <v>29</v>
       </c>
       <c r="G24" s="23"/>
-      <c r="H24" s="50"/>
+      <c r="H24" s="48"/>
       <c r="I24" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="J24" s="49"/>
+      <c r="J24" s="47"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
@@ -1883,34 +1905,34 @@
       <c r="F25" s="21"/>
       <c r="G25" s="10"/>
       <c r="H25" s="5"/>
-      <c r="I25" s="88" t="s">
+      <c r="I25" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="J25" s="83"/>
+      <c r="J25" s="64"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
       <c r="C26" s="5"/>
-      <c r="D26" s="87"/>
+      <c r="D26" s="69"/>
       <c r="E26" s="4"/>
       <c r="F26" s="21"/>
       <c r="G26" s="10"/>
       <c r="H26" s="5"/>
-      <c r="I26" s="88"/>
-      <c r="J26" s="83"/>
+      <c r="I26" s="71"/>
+      <c r="J26" s="64"/>
     </row>
     <row r="27" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="4"/>
       <c r="C27" s="5"/>
-      <c r="D27" s="87"/>
+      <c r="D27" s="69"/>
       <c r="E27" s="4"/>
       <c r="F27" s="21"/>
       <c r="G27" s="10"/>
       <c r="H27" s="5"/>
-      <c r="I27" s="89"/>
-      <c r="J27" s="84"/>
+      <c r="I27" s="72"/>
+      <c r="J27" s="65"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
@@ -1921,10 +1943,10 @@
       <c r="F28" s="21"/>
       <c r="G28" s="10"/>
       <c r="H28" s="5"/>
-      <c r="I28" s="90" t="s">
+      <c r="I28" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="J28" s="83"/>
+      <c r="J28" s="64"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
@@ -1935,8 +1957,8 @@
       <c r="F29" s="21"/>
       <c r="G29" s="10"/>
       <c r="H29" s="5"/>
-      <c r="I29" s="88"/>
-      <c r="J29" s="83"/>
+      <c r="I29" s="71"/>
+      <c r="J29" s="64"/>
     </row>
     <row r="30" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
@@ -1947,8 +1969,8 @@
       <c r="F30" s="21"/>
       <c r="G30" s="10"/>
       <c r="H30" s="5"/>
-      <c r="I30" s="89"/>
-      <c r="J30" s="84"/>
+      <c r="I30" s="72"/>
+      <c r="J30" s="65"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
@@ -1959,34 +1981,34 @@
       <c r="F31" s="21"/>
       <c r="G31" s="10"/>
       <c r="H31" s="5"/>
-      <c r="I31" s="90" t="s">
+      <c r="I31" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="J31" s="83"/>
+      <c r="J31" s="64"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="4"/>
       <c r="C32" s="5"/>
-      <c r="D32" s="87"/>
+      <c r="D32" s="69"/>
       <c r="E32" s="4"/>
       <c r="F32" s="21"/>
       <c r="G32" s="10"/>
       <c r="H32" s="5"/>
-      <c r="I32" s="88"/>
-      <c r="J32" s="83"/>
+      <c r="I32" s="71"/>
+      <c r="J32" s="64"/>
     </row>
     <row r="33" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
-      <c r="D33" s="87"/>
+      <c r="D33" s="69"/>
       <c r="E33" s="4"/>
       <c r="F33" s="21"/>
       <c r="G33" s="10"/>
       <c r="H33" s="5"/>
-      <c r="I33" s="89"/>
-      <c r="J33" s="84"/>
+      <c r="I33" s="72"/>
+      <c r="J33" s="65"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
@@ -1997,10 +2019,10 @@
       <c r="F34" s="21"/>
       <c r="G34" s="10"/>
       <c r="H34" s="5"/>
-      <c r="I34" s="90" t="s">
+      <c r="I34" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="J34" s="83"/>
+      <c r="J34" s="64"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
@@ -2011,8 +2033,8 @@
       <c r="F35" s="21"/>
       <c r="G35" s="10"/>
       <c r="H35" s="5"/>
-      <c r="I35" s="88"/>
-      <c r="J35" s="83"/>
+      <c r="I35" s="71"/>
+      <c r="J35" s="64"/>
     </row>
     <row r="36" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
@@ -2023,8 +2045,8 @@
       <c r="F36" s="21"/>
       <c r="G36" s="10"/>
       <c r="H36" s="5"/>
-      <c r="I36" s="89"/>
-      <c r="J36" s="84"/>
+      <c r="I36" s="72"/>
+      <c r="J36" s="65"/>
     </row>
     <row r="37" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
@@ -2035,10 +2057,10 @@
       <c r="F37" s="3"/>
       <c r="G37" s="4"/>
       <c r="H37" s="5"/>
-      <c r="I37" s="90" t="s">
+      <c r="I37" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="J37" s="83"/>
+      <c r="J37" s="64"/>
     </row>
     <row r="38" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="15"/>
@@ -2047,42 +2069,42 @@
       <c r="D38" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="E38" s="51"/>
+      <c r="E38" s="49"/>
       <c r="F38" s="19"/>
       <c r="G38" s="10"/>
       <c r="H38" s="18"/>
-      <c r="I38" s="88"/>
-      <c r="J38" s="83"/>
+      <c r="I38" s="71"/>
+      <c r="J38" s="64"/>
     </row>
     <row r="39" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="93"/>
-      <c r="C39" s="94"/>
+      <c r="B39" s="62"/>
+      <c r="C39" s="63"/>
       <c r="D39" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="E39" s="52"/>
+      <c r="E39" s="50"/>
       <c r="F39" s="15"/>
       <c r="G39" s="22"/>
       <c r="H39" s="20"/>
-      <c r="I39" s="89"/>
-      <c r="J39" s="84"/>
+      <c r="I39" s="72"/>
+      <c r="J39" s="65"/>
     </row>
     <row r="40" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="80" t="s">
+      <c r="A40" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="B40" s="81"/>
-      <c r="C40" s="81"/>
-      <c r="D40" s="81"/>
-      <c r="E40" s="81"/>
-      <c r="F40" s="81"/>
-      <c r="G40" s="81"/>
-      <c r="H40" s="81"/>
-      <c r="I40" s="81"/>
-      <c r="J40" s="82"/>
+      <c r="B40" s="67"/>
+      <c r="C40" s="67"/>
+      <c r="D40" s="67"/>
+      <c r="E40" s="67"/>
+      <c r="F40" s="67"/>
+      <c r="G40" s="67"/>
+      <c r="H40" s="67"/>
+      <c r="I40" s="67"/>
+      <c r="J40" s="68"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
@@ -2233,10 +2255,10 @@
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="2"/>
-      <c r="E53" s="90" t="s">
+      <c r="E53" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="F53" s="95"/>
+      <c r="F53" s="73"/>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
@@ -2247,8 +2269,8 @@
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="5"/>
-      <c r="E54" s="88"/>
-      <c r="F54" s="83"/>
+      <c r="E54" s="71"/>
+      <c r="F54" s="64"/>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
@@ -2259,8 +2281,8 @@
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="5"/>
-      <c r="E55" s="89"/>
-      <c r="F55" s="84"/>
+      <c r="E55" s="72"/>
+      <c r="F55" s="65"/>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
@@ -2271,10 +2293,10 @@
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="5"/>
-      <c r="E56" s="90" t="s">
+      <c r="E56" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="F56" s="95"/>
+      <c r="F56" s="73"/>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
@@ -2285,8 +2307,8 @@
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="5"/>
-      <c r="E57" s="88"/>
-      <c r="F57" s="83"/>
+      <c r="E57" s="71"/>
+      <c r="F57" s="64"/>
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
@@ -2297,8 +2319,8 @@
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="5"/>
-      <c r="E58" s="89"/>
-      <c r="F58" s="84"/>
+      <c r="E58" s="72"/>
+      <c r="F58" s="65"/>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
@@ -2309,10 +2331,10 @@
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="5"/>
-      <c r="E59" s="90" t="s">
+      <c r="E59" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="F59" s="95"/>
+      <c r="F59" s="73"/>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
@@ -2323,8 +2345,8 @@
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="5"/>
-      <c r="E60" s="88"/>
-      <c r="F60" s="83"/>
+      <c r="E60" s="71"/>
+      <c r="F60" s="64"/>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
@@ -2335,8 +2357,8 @@
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="5"/>
-      <c r="E61" s="89"/>
-      <c r="F61" s="84"/>
+      <c r="E61" s="72"/>
+      <c r="F61" s="65"/>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
@@ -2347,8 +2369,8 @@
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="5"/>
-      <c r="E62" s="54"/>
-      <c r="F62" s="53"/>
+      <c r="E62" s="52"/>
+      <c r="F62" s="51"/>
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
       <c r="I62" s="4"/>
@@ -2359,12 +2381,12 @@
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
       <c r="D63" s="8"/>
-      <c r="E63" s="55"/>
-      <c r="F63" s="56"/>
+      <c r="E63" s="53"/>
+      <c r="F63" s="54"/>
       <c r="G63" s="7"/>
       <c r="H63" s="7"/>
-      <c r="I63" s="91"/>
-      <c r="J63" s="92"/>
+      <c r="I63" s="60"/>
+      <c r="J63" s="61"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
@@ -2413,30 +2435,6 @@
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <dataConsolidate/>
   <mergeCells count="39">
-    <mergeCell ref="I63:J63"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="J37:J39"/>
-    <mergeCell ref="A40:J40"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="I37:I39"/>
-    <mergeCell ref="E53:E55"/>
-    <mergeCell ref="E56:E58"/>
-    <mergeCell ref="E59:E61"/>
-    <mergeCell ref="F53:F55"/>
-    <mergeCell ref="F56:F58"/>
-    <mergeCell ref="F59:F61"/>
-    <mergeCell ref="J34:J36"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="I25:I27"/>
-    <mergeCell ref="I28:I30"/>
-    <mergeCell ref="J25:J27"/>
-    <mergeCell ref="I31:I33"/>
-    <mergeCell ref="I34:I36"/>
-    <mergeCell ref="J28:J30"/>
-    <mergeCell ref="J31:J33"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A23:J23"/>
     <mergeCell ref="I2:J2"/>
@@ -2452,6 +2450,30 @@
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="A22:B22"/>
+    <mergeCell ref="I28:I30"/>
+    <mergeCell ref="J25:J27"/>
+    <mergeCell ref="I31:I33"/>
+    <mergeCell ref="I34:I36"/>
+    <mergeCell ref="J28:J30"/>
+    <mergeCell ref="J31:J33"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="I25:I27"/>
+    <mergeCell ref="I63:J63"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="J37:J39"/>
+    <mergeCell ref="A40:J40"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="I37:I39"/>
+    <mergeCell ref="E53:E55"/>
+    <mergeCell ref="E56:E58"/>
+    <mergeCell ref="E59:E61"/>
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="F56:F58"/>
+    <mergeCell ref="F59:F61"/>
+    <mergeCell ref="J34:J36"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2473,39 +2495,39 @@
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="57"/>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
+      <c r="A1" s="55"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="57"/>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
+      <c r="A3" s="55"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="57"/>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
+      <c r="A4" s="55"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="57"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -2526,39 +2548,39 @@
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="57"/>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
+      <c r="A1" s="55"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="57"/>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
+      <c r="A3" s="55"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="57"/>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
+      <c r="A4" s="55"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="57"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
null cell kontrolü eklendi
</commit_message>
<xml_diff>
--- a/WebApplication1/Forms/03_EgzozValf.xlsx
+++ b/WebApplication1/Forms/03_EgzozValf.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>VESSEL</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>De-Mounted fr Cyl.</t>
+  </si>
+  <si>
+    <t>{NN}</t>
   </si>
 </sst>
 </file>
@@ -540,19 +543,109 @@
     <xf numFmtId="1" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -562,123 +655,33 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1539,7 +1542,7 @@
   <dimension ref="A1:P76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1550,71 +1553,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
-      <c r="J1" s="82"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="62"/>
     </row>
     <row r="2" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="88"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="76" t="s">
+      <c r="B2" s="68"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="77"/>
-      <c r="F2" s="93" t="s">
+      <c r="E2" s="71"/>
+      <c r="F2" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="94"/>
+      <c r="G2" s="76"/>
       <c r="H2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="86"/>
-      <c r="J2" s="87"/>
+      <c r="I2" s="66" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="67"/>
     </row>
     <row r="3" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="59"/>
+      <c r="B3" s="59" t="s">
+        <v>37</v>
+      </c>
       <c r="C3" s="43" t="s">
         <v>35</v>
       </c>
       <c r="D3" s="56"/>
-      <c r="E3" s="95" t="s">
+      <c r="E3" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="96"/>
+      <c r="F3" s="78"/>
       <c r="G3" s="57"/>
       <c r="H3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="100"/>
-      <c r="J3" s="101"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="86"/>
     </row>
     <row r="4" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="90" t="s">
+      <c r="A4" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="91"/>
-      <c r="C4" s="91"/>
-      <c r="D4" s="92"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="74"/>
       <c r="E4" s="58"/>
-      <c r="F4" s="76" t="s">
+      <c r="F4" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="77"/>
+      <c r="G4" s="71"/>
       <c r="H4" s="58"/>
       <c r="I4" s="23" t="s">
         <v>5</v>
@@ -1622,20 +1629,20 @@
       <c r="J4" s="58"/>
     </row>
     <row r="5" spans="1:16" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="66" t="s">
+      <c r="A5" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="97" t="s">
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="98"/>
-      <c r="G5" s="98"/>
-      <c r="H5" s="98"/>
-      <c r="I5" s="98"/>
-      <c r="J5" s="99"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="80"/>
+      <c r="J5" s="81"/>
       <c r="K5" s="44"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -1801,8 +1808,10 @@
       <c r="A19" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="74"/>
-      <c r="C19" s="75"/>
+      <c r="B19" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="88"/>
       <c r="D19" s="28" t="s">
         <v>31</v>
       </c>
@@ -1828,10 +1837,10 @@
       <c r="J20" s="5"/>
     </row>
     <row r="21" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="95" t="s">
+      <c r="A21" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="96"/>
+      <c r="B21" s="78"/>
       <c r="C21" s="46"/>
       <c r="D21" s="33" t="s">
         <v>33</v>
@@ -1844,44 +1853,44 @@
       <c r="J21" s="8"/>
     </row>
     <row r="22" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="95" t="s">
+      <c r="A22" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="96"/>
+      <c r="B22" s="78"/>
       <c r="C22" s="46"/>
       <c r="D22" s="47"/>
-      <c r="E22" s="76" t="s">
+      <c r="E22" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="77"/>
+      <c r="F22" s="71"/>
       <c r="G22" s="45"/>
       <c r="H22" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I22" s="78"/>
-      <c r="J22" s="79"/>
+      <c r="I22" s="94"/>
+      <c r="J22" s="95"/>
     </row>
     <row r="23" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="83" t="s">
+      <c r="A23" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="84"/>
-      <c r="C23" s="84"/>
-      <c r="D23" s="84"/>
-      <c r="E23" s="84"/>
-      <c r="F23" s="84"/>
-      <c r="G23" s="84"/>
-      <c r="H23" s="84"/>
-      <c r="I23" s="84"/>
-      <c r="J23" s="85"/>
+      <c r="B23" s="64"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="64"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="64"/>
+      <c r="H23" s="64"/>
+      <c r="I23" s="64"/>
+      <c r="J23" s="65"/>
       <c r="L23" s="31"/>
     </row>
     <row r="24" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="74"/>
-      <c r="C24" s="75"/>
+      <c r="B24" s="87"/>
+      <c r="C24" s="88"/>
       <c r="D24" s="34" t="s">
         <v>32</v>
       </c>
@@ -1905,34 +1914,34 @@
       <c r="F25" s="21"/>
       <c r="G25" s="10"/>
       <c r="H25" s="5"/>
-      <c r="I25" s="71" t="s">
+      <c r="I25" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="J25" s="64"/>
+      <c r="J25" s="92"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
       <c r="C26" s="5"/>
-      <c r="D26" s="69"/>
+      <c r="D26" s="96"/>
       <c r="E26" s="4"/>
       <c r="F26" s="21"/>
       <c r="G26" s="10"/>
       <c r="H26" s="5"/>
-      <c r="I26" s="71"/>
-      <c r="J26" s="64"/>
+      <c r="I26" s="90"/>
+      <c r="J26" s="92"/>
     </row>
     <row r="27" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="4"/>
       <c r="C27" s="5"/>
-      <c r="D27" s="69"/>
+      <c r="D27" s="96"/>
       <c r="E27" s="4"/>
       <c r="F27" s="21"/>
       <c r="G27" s="10"/>
       <c r="H27" s="5"/>
-      <c r="I27" s="72"/>
-      <c r="J27" s="65"/>
+      <c r="I27" s="91"/>
+      <c r="J27" s="93"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
@@ -1943,10 +1952,10 @@
       <c r="F28" s="21"/>
       <c r="G28" s="10"/>
       <c r="H28" s="5"/>
-      <c r="I28" s="70" t="s">
+      <c r="I28" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="J28" s="64"/>
+      <c r="J28" s="92"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
@@ -1957,8 +1966,8 @@
       <c r="F29" s="21"/>
       <c r="G29" s="10"/>
       <c r="H29" s="5"/>
-      <c r="I29" s="71"/>
-      <c r="J29" s="64"/>
+      <c r="I29" s="90"/>
+      <c r="J29" s="92"/>
     </row>
     <row r="30" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
@@ -1969,8 +1978,8 @@
       <c r="F30" s="21"/>
       <c r="G30" s="10"/>
       <c r="H30" s="5"/>
-      <c r="I30" s="72"/>
-      <c r="J30" s="65"/>
+      <c r="I30" s="91"/>
+      <c r="J30" s="93"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
@@ -1981,34 +1990,34 @@
       <c r="F31" s="21"/>
       <c r="G31" s="10"/>
       <c r="H31" s="5"/>
-      <c r="I31" s="70" t="s">
+      <c r="I31" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="J31" s="64"/>
+      <c r="J31" s="92"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="4"/>
       <c r="C32" s="5"/>
-      <c r="D32" s="69"/>
+      <c r="D32" s="96"/>
       <c r="E32" s="4"/>
       <c r="F32" s="21"/>
       <c r="G32" s="10"/>
       <c r="H32" s="5"/>
-      <c r="I32" s="71"/>
-      <c r="J32" s="64"/>
+      <c r="I32" s="90"/>
+      <c r="J32" s="92"/>
     </row>
     <row r="33" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
-      <c r="D33" s="69"/>
+      <c r="D33" s="96"/>
       <c r="E33" s="4"/>
       <c r="F33" s="21"/>
       <c r="G33" s="10"/>
       <c r="H33" s="5"/>
-      <c r="I33" s="72"/>
-      <c r="J33" s="65"/>
+      <c r="I33" s="91"/>
+      <c r="J33" s="93"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
@@ -2019,10 +2028,10 @@
       <c r="F34" s="21"/>
       <c r="G34" s="10"/>
       <c r="H34" s="5"/>
-      <c r="I34" s="70" t="s">
+      <c r="I34" s="89" t="s">
         <v>17</v>
       </c>
-      <c r="J34" s="64"/>
+      <c r="J34" s="92"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
@@ -2033,8 +2042,8 @@
       <c r="F35" s="21"/>
       <c r="G35" s="10"/>
       <c r="H35" s="5"/>
-      <c r="I35" s="71"/>
-      <c r="J35" s="64"/>
+      <c r="I35" s="90"/>
+      <c r="J35" s="92"/>
     </row>
     <row r="36" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
@@ -2045,8 +2054,8 @@
       <c r="F36" s="21"/>
       <c r="G36" s="10"/>
       <c r="H36" s="5"/>
-      <c r="I36" s="72"/>
-      <c r="J36" s="65"/>
+      <c r="I36" s="91"/>
+      <c r="J36" s="93"/>
     </row>
     <row r="37" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
@@ -2057,10 +2066,10 @@
       <c r="F37" s="3"/>
       <c r="G37" s="4"/>
       <c r="H37" s="5"/>
-      <c r="I37" s="70" t="s">
+      <c r="I37" s="89" t="s">
         <v>18</v>
       </c>
-      <c r="J37" s="64"/>
+      <c r="J37" s="92"/>
     </row>
     <row r="38" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="15"/>
@@ -2073,15 +2082,15 @@
       <c r="F38" s="19"/>
       <c r="G38" s="10"/>
       <c r="H38" s="18"/>
-      <c r="I38" s="71"/>
-      <c r="J38" s="64"/>
+      <c r="I38" s="90"/>
+      <c r="J38" s="92"/>
     </row>
     <row r="39" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="62"/>
-      <c r="C39" s="63"/>
+      <c r="B39" s="99"/>
+      <c r="C39" s="100"/>
       <c r="D39" s="26" t="s">
         <v>24</v>
       </c>
@@ -2089,22 +2098,22 @@
       <c r="F39" s="15"/>
       <c r="G39" s="22"/>
       <c r="H39" s="20"/>
-      <c r="I39" s="72"/>
-      <c r="J39" s="65"/>
+      <c r="I39" s="91"/>
+      <c r="J39" s="93"/>
     </row>
     <row r="40" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="66" t="s">
+      <c r="A40" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="B40" s="67"/>
-      <c r="C40" s="67"/>
-      <c r="D40" s="67"/>
-      <c r="E40" s="67"/>
-      <c r="F40" s="67"/>
-      <c r="G40" s="67"/>
-      <c r="H40" s="67"/>
-      <c r="I40" s="67"/>
-      <c r="J40" s="68"/>
+      <c r="B40" s="83"/>
+      <c r="C40" s="83"/>
+      <c r="D40" s="83"/>
+      <c r="E40" s="83"/>
+      <c r="F40" s="83"/>
+      <c r="G40" s="83"/>
+      <c r="H40" s="83"/>
+      <c r="I40" s="83"/>
+      <c r="J40" s="84"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
@@ -2255,10 +2264,10 @@
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="2"/>
-      <c r="E53" s="70" t="s">
+      <c r="E53" s="89" t="s">
         <v>25</v>
       </c>
-      <c r="F53" s="73"/>
+      <c r="F53" s="101"/>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
@@ -2269,8 +2278,8 @@
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="5"/>
-      <c r="E54" s="71"/>
-      <c r="F54" s="64"/>
+      <c r="E54" s="90"/>
+      <c r="F54" s="92"/>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
@@ -2281,8 +2290,8 @@
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="5"/>
-      <c r="E55" s="72"/>
-      <c r="F55" s="65"/>
+      <c r="E55" s="91"/>
+      <c r="F55" s="93"/>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
@@ -2293,10 +2302,10 @@
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="5"/>
-      <c r="E56" s="70" t="s">
+      <c r="E56" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="F56" s="73"/>
+      <c r="F56" s="101"/>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
@@ -2307,8 +2316,8 @@
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="5"/>
-      <c r="E57" s="71"/>
-      <c r="F57" s="64"/>
+      <c r="E57" s="90"/>
+      <c r="F57" s="92"/>
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
@@ -2319,8 +2328,8 @@
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="5"/>
-      <c r="E58" s="72"/>
-      <c r="F58" s="65"/>
+      <c r="E58" s="91"/>
+      <c r="F58" s="93"/>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
@@ -2331,10 +2340,10 @@
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="5"/>
-      <c r="E59" s="70" t="s">
+      <c r="E59" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="F59" s="73"/>
+      <c r="F59" s="101"/>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
@@ -2345,8 +2354,8 @@
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="5"/>
-      <c r="E60" s="71"/>
-      <c r="F60" s="64"/>
+      <c r="E60" s="90"/>
+      <c r="F60" s="92"/>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
@@ -2357,8 +2366,8 @@
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="5"/>
-      <c r="E61" s="72"/>
-      <c r="F61" s="65"/>
+      <c r="E61" s="91"/>
+      <c r="F61" s="93"/>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
@@ -2385,8 +2394,8 @@
       <c r="F63" s="54"/>
       <c r="G63" s="7"/>
       <c r="H63" s="7"/>
-      <c r="I63" s="60"/>
-      <c r="J63" s="61"/>
+      <c r="I63" s="97"/>
+      <c r="J63" s="98"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
@@ -2435,6 +2444,30 @@
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <dataConsolidate/>
   <mergeCells count="39">
+    <mergeCell ref="I63:J63"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="J37:J39"/>
+    <mergeCell ref="A40:J40"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="I37:I39"/>
+    <mergeCell ref="E53:E55"/>
+    <mergeCell ref="E56:E58"/>
+    <mergeCell ref="E59:E61"/>
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="F56:F58"/>
+    <mergeCell ref="F59:F61"/>
+    <mergeCell ref="J34:J36"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="I25:I27"/>
+    <mergeCell ref="I28:I30"/>
+    <mergeCell ref="J25:J27"/>
+    <mergeCell ref="I31:I33"/>
+    <mergeCell ref="I34:I36"/>
+    <mergeCell ref="J28:J30"/>
+    <mergeCell ref="J31:J33"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A23:J23"/>
     <mergeCell ref="I2:J2"/>
@@ -2450,30 +2483,6 @@
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="A22:B22"/>
-    <mergeCell ref="I28:I30"/>
-    <mergeCell ref="J25:J27"/>
-    <mergeCell ref="I31:I33"/>
-    <mergeCell ref="I34:I36"/>
-    <mergeCell ref="J28:J30"/>
-    <mergeCell ref="J31:J33"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="I25:I27"/>
-    <mergeCell ref="I63:J63"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="J37:J39"/>
-    <mergeCell ref="A40:J40"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="I37:I39"/>
-    <mergeCell ref="E53:E55"/>
-    <mergeCell ref="E56:E58"/>
-    <mergeCell ref="E59:E61"/>
-    <mergeCell ref="F53:F55"/>
-    <mergeCell ref="F56:F58"/>
-    <mergeCell ref="F59:F61"/>
-    <mergeCell ref="J34:J36"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
ship particular cellerin otomatik doldurulması
</commit_message>
<xml_diff>
--- a/WebApplication1/Forms/03_EgzozValf.xlsx
+++ b/WebApplication1/Forms/03_EgzozValf.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>VESSEL</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>{NN}</t>
+  </si>
+  <si>
+    <t>{VesselName}</t>
+  </si>
+  <si>
+    <t>{BuilderNo}</t>
   </si>
 </sst>
 </file>
@@ -408,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -621,14 +627,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1542,7 +1540,7 @@
   <dimension ref="A1:P76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+      <selection activeCell="I3" sqref="I3:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1570,7 +1568,9 @@
       <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="68"/>
+      <c r="B2" s="68" t="s">
+        <v>38</v>
+      </c>
       <c r="C2" s="69"/>
       <c r="D2" s="70" t="s">
         <v>1</v>
@@ -1607,8 +1607,10 @@
       <c r="H3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="85"/>
-      <c r="J3" s="86"/>
+      <c r="I3" s="68" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="69"/>
     </row>
     <row r="4" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="72" t="s">
@@ -1808,10 +1810,10 @@
       <c r="A19" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="87" t="s">
+      <c r="B19" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="88"/>
+      <c r="C19" s="86"/>
       <c r="D19" s="28" t="s">
         <v>31</v>
       </c>
@@ -1867,8 +1869,8 @@
       <c r="H22" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I22" s="94"/>
-      <c r="J22" s="95"/>
+      <c r="I22" s="92"/>
+      <c r="J22" s="93"/>
     </row>
     <row r="23" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="63" t="s">
@@ -1889,8 +1891,8 @@
       <c r="A24" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="87"/>
-      <c r="C24" s="88"/>
+      <c r="B24" s="85"/>
+      <c r="C24" s="86"/>
       <c r="D24" s="34" t="s">
         <v>32</v>
       </c>
@@ -1914,34 +1916,34 @@
       <c r="F25" s="21"/>
       <c r="G25" s="10"/>
       <c r="H25" s="5"/>
-      <c r="I25" s="90" t="s">
+      <c r="I25" s="88" t="s">
         <v>14</v>
       </c>
-      <c r="J25" s="92"/>
+      <c r="J25" s="90"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
       <c r="C26" s="5"/>
-      <c r="D26" s="96"/>
+      <c r="D26" s="94"/>
       <c r="E26" s="4"/>
       <c r="F26" s="21"/>
       <c r="G26" s="10"/>
       <c r="H26" s="5"/>
-      <c r="I26" s="90"/>
-      <c r="J26" s="92"/>
+      <c r="I26" s="88"/>
+      <c r="J26" s="90"/>
     </row>
     <row r="27" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="4"/>
       <c r="C27" s="5"/>
-      <c r="D27" s="96"/>
+      <c r="D27" s="94"/>
       <c r="E27" s="4"/>
       <c r="F27" s="21"/>
       <c r="G27" s="10"/>
       <c r="H27" s="5"/>
-      <c r="I27" s="91"/>
-      <c r="J27" s="93"/>
+      <c r="I27" s="89"/>
+      <c r="J27" s="91"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
@@ -1952,10 +1954,10 @@
       <c r="F28" s="21"/>
       <c r="G28" s="10"/>
       <c r="H28" s="5"/>
-      <c r="I28" s="89" t="s">
+      <c r="I28" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="J28" s="92"/>
+      <c r="J28" s="90"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
@@ -1966,8 +1968,8 @@
       <c r="F29" s="21"/>
       <c r="G29" s="10"/>
       <c r="H29" s="5"/>
-      <c r="I29" s="90"/>
-      <c r="J29" s="92"/>
+      <c r="I29" s="88"/>
+      <c r="J29" s="90"/>
     </row>
     <row r="30" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
@@ -1978,8 +1980,8 @@
       <c r="F30" s="21"/>
       <c r="G30" s="10"/>
       <c r="H30" s="5"/>
-      <c r="I30" s="91"/>
-      <c r="J30" s="93"/>
+      <c r="I30" s="89"/>
+      <c r="J30" s="91"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
@@ -1990,34 +1992,34 @@
       <c r="F31" s="21"/>
       <c r="G31" s="10"/>
       <c r="H31" s="5"/>
-      <c r="I31" s="89" t="s">
+      <c r="I31" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="J31" s="92"/>
+      <c r="J31" s="90"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="4"/>
       <c r="C32" s="5"/>
-      <c r="D32" s="96"/>
+      <c r="D32" s="94"/>
       <c r="E32" s="4"/>
       <c r="F32" s="21"/>
       <c r="G32" s="10"/>
       <c r="H32" s="5"/>
-      <c r="I32" s="90"/>
-      <c r="J32" s="92"/>
+      <c r="I32" s="88"/>
+      <c r="J32" s="90"/>
     </row>
     <row r="33" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
-      <c r="D33" s="96"/>
+      <c r="D33" s="94"/>
       <c r="E33" s="4"/>
       <c r="F33" s="21"/>
       <c r="G33" s="10"/>
       <c r="H33" s="5"/>
-      <c r="I33" s="91"/>
-      <c r="J33" s="93"/>
+      <c r="I33" s="89"/>
+      <c r="J33" s="91"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
@@ -2028,10 +2030,10 @@
       <c r="F34" s="21"/>
       <c r="G34" s="10"/>
       <c r="H34" s="5"/>
-      <c r="I34" s="89" t="s">
+      <c r="I34" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="J34" s="92"/>
+      <c r="J34" s="90"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
@@ -2042,8 +2044,8 @@
       <c r="F35" s="21"/>
       <c r="G35" s="10"/>
       <c r="H35" s="5"/>
-      <c r="I35" s="90"/>
-      <c r="J35" s="92"/>
+      <c r="I35" s="88"/>
+      <c r="J35" s="90"/>
     </row>
     <row r="36" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
@@ -2054,8 +2056,8 @@
       <c r="F36" s="21"/>
       <c r="G36" s="10"/>
       <c r="H36" s="5"/>
-      <c r="I36" s="91"/>
-      <c r="J36" s="93"/>
+      <c r="I36" s="89"/>
+      <c r="J36" s="91"/>
     </row>
     <row r="37" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
@@ -2066,10 +2068,10 @@
       <c r="F37" s="3"/>
       <c r="G37" s="4"/>
       <c r="H37" s="5"/>
-      <c r="I37" s="89" t="s">
+      <c r="I37" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="J37" s="92"/>
+      <c r="J37" s="90"/>
     </row>
     <row r="38" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="15"/>
@@ -2082,15 +2084,15 @@
       <c r="F38" s="19"/>
       <c r="G38" s="10"/>
       <c r="H38" s="18"/>
-      <c r="I38" s="90"/>
-      <c r="J38" s="92"/>
+      <c r="I38" s="88"/>
+      <c r="J38" s="90"/>
     </row>
     <row r="39" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="99"/>
-      <c r="C39" s="100"/>
+      <c r="B39" s="97"/>
+      <c r="C39" s="98"/>
       <c r="D39" s="26" t="s">
         <v>24</v>
       </c>
@@ -2098,8 +2100,8 @@
       <c r="F39" s="15"/>
       <c r="G39" s="22"/>
       <c r="H39" s="20"/>
-      <c r="I39" s="91"/>
-      <c r="J39" s="93"/>
+      <c r="I39" s="89"/>
+      <c r="J39" s="91"/>
     </row>
     <row r="40" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="82" t="s">
@@ -2264,10 +2266,10 @@
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="2"/>
-      <c r="E53" s="89" t="s">
+      <c r="E53" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="F53" s="101"/>
+      <c r="F53" s="99"/>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
@@ -2278,8 +2280,8 @@
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="5"/>
-      <c r="E54" s="90"/>
-      <c r="F54" s="92"/>
+      <c r="E54" s="88"/>
+      <c r="F54" s="90"/>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
@@ -2290,8 +2292,8 @@
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="5"/>
-      <c r="E55" s="91"/>
-      <c r="F55" s="93"/>
+      <c r="E55" s="89"/>
+      <c r="F55" s="91"/>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
@@ -2302,10 +2304,10 @@
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="5"/>
-      <c r="E56" s="89" t="s">
+      <c r="E56" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="F56" s="101"/>
+      <c r="F56" s="99"/>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
@@ -2316,8 +2318,8 @@
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="5"/>
-      <c r="E57" s="90"/>
-      <c r="F57" s="92"/>
+      <c r="E57" s="88"/>
+      <c r="F57" s="90"/>
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
@@ -2328,8 +2330,8 @@
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="5"/>
-      <c r="E58" s="91"/>
-      <c r="F58" s="93"/>
+      <c r="E58" s="89"/>
+      <c r="F58" s="91"/>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
@@ -2340,10 +2342,10 @@
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="5"/>
-      <c r="E59" s="89" t="s">
+      <c r="E59" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="F59" s="101"/>
+      <c r="F59" s="99"/>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
@@ -2354,8 +2356,8 @@
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="5"/>
-      <c r="E60" s="90"/>
-      <c r="F60" s="92"/>
+      <c r="E60" s="88"/>
+      <c r="F60" s="90"/>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
@@ -2366,8 +2368,8 @@
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="5"/>
-      <c r="E61" s="91"/>
-      <c r="F61" s="93"/>
+      <c r="E61" s="89"/>
+      <c r="F61" s="91"/>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
@@ -2394,8 +2396,8 @@
       <c r="F63" s="54"/>
       <c r="G63" s="7"/>
       <c r="H63" s="7"/>
-      <c r="I63" s="97"/>
-      <c r="J63" s="98"/>
+      <c r="I63" s="95"/>
+      <c r="J63" s="96"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>

</xml_diff>

<commit_message>
excel üzerinde format düzeltmesi
</commit_message>
<xml_diff>
--- a/WebApplication1/Forms/03_EgzozValf.xlsx
+++ b/WebApplication1/Forms/03_EgzozValf.xlsx
@@ -414,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -428,10 +428,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -464,90 +460,105 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -604,27 +615,27 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -636,50 +647,59 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1551,399 +1571,399 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
-      <c r="J1" s="82"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="90"/>
     </row>
     <row r="2" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="96" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="89"/>
-      <c r="D2" s="76" t="s">
+      <c r="C2" s="97"/>
+      <c r="D2" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="77"/>
-      <c r="F2" s="93" t="s">
+      <c r="E2" s="85"/>
+      <c r="F2" s="101" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="94"/>
-      <c r="H2" s="24" t="s">
+      <c r="G2" s="102"/>
+      <c r="H2" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="86" t="s">
+      <c r="I2" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="87"/>
+      <c r="J2" s="95"/>
     </row>
     <row r="3" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="42" t="s">
         <v>37</v>
       </c>
       <c r="C3" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="56"/>
-      <c r="E3" s="95" t="s">
+      <c r="D3" s="42"/>
+      <c r="E3" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="96"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="12" t="s">
+      <c r="F3" s="104"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="88" t="s">
+      <c r="I3" s="96" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="89"/>
+      <c r="J3" s="97"/>
     </row>
     <row r="4" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="90" t="s">
+      <c r="A4" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="91"/>
-      <c r="C4" s="91"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="76" t="s">
+      <c r="B4" s="99"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="77"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="23" t="s">
+      <c r="G4" s="85"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="58"/>
+      <c r="J4" s="46"/>
     </row>
     <row r="5" spans="1:16" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="66" t="s">
+      <c r="A5" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="97" t="s">
+      <c r="B5" s="109"/>
+      <c r="C5" s="109"/>
+      <c r="D5" s="110"/>
+      <c r="E5" s="105" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="98"/>
-      <c r="G5" s="98"/>
-      <c r="H5" s="98"/>
-      <c r="I5" s="98"/>
-      <c r="J5" s="99"/>
-      <c r="K5" s="44"/>
+      <c r="F5" s="106"/>
+      <c r="G5" s="106"/>
+      <c r="H5" s="106"/>
+      <c r="I5" s="106"/>
+      <c r="J5" s="107"/>
+      <c r="K5" s="29"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="36"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="42"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="53"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="5"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="56"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="5"/>
-      <c r="P8" s="16"/>
+      <c r="A8" s="54"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="56"/>
+      <c r="P8" s="14"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="5"/>
-      <c r="P9" s="16"/>
+      <c r="A9" s="54"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="56"/>
+      <c r="P9" s="14"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="5"/>
+      <c r="A10" s="54"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="56"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="5"/>
+      <c r="A11" s="54"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="55"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="56"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="5"/>
+      <c r="A12" s="54"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="55"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="56"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="5"/>
+      <c r="A13" s="54"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="56"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="5"/>
+      <c r="A14" s="54"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="55"/>
+      <c r="I14" s="55"/>
+      <c r="J14" s="56"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="5"/>
+      <c r="A15" s="54"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="55"/>
+      <c r="I15" s="55"/>
+      <c r="J15" s="56"/>
       <c r="L15" s="4"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="5"/>
+      <c r="A16" s="54"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="55"/>
+      <c r="H16" s="55"/>
+      <c r="I16" s="55"/>
+      <c r="J16" s="56"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="5"/>
+      <c r="A17" s="54"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="55"/>
+      <c r="I17" s="55"/>
+      <c r="J17" s="56"/>
     </row>
     <row r="18" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="5"/>
+      <c r="A18" s="58"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="54"/>
+      <c r="F18" s="55"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="55"/>
+      <c r="I18" s="55"/>
+      <c r="J18" s="56"/>
     </row>
     <row r="19" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="74" t="s">
+      <c r="B19" s="96" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="75"/>
-      <c r="D19" s="28" t="s">
+      <c r="C19" s="97"/>
+      <c r="D19" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="5"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="55"/>
+      <c r="G19" s="55"/>
+      <c r="H19" s="55"/>
+      <c r="I19" s="55"/>
+      <c r="J19" s="56"/>
     </row>
     <row r="20" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="5"/>
+      <c r="B20" s="64"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="66"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="55"/>
+      <c r="I20" s="55"/>
+      <c r="J20" s="56"/>
     </row>
     <row r="21" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="95" t="s">
+      <c r="A21" s="103" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="96"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="33" t="s">
+      <c r="B21" s="104"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="6"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="8"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="59"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="59"/>
+      <c r="J21" s="60"/>
     </row>
     <row r="22" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="95" t="s">
+      <c r="A22" s="103" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="96"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="76" t="s">
+      <c r="B22" s="104"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="77"/>
-      <c r="G22" s="45"/>
-      <c r="H22" s="24" t="s">
+      <c r="F22" s="85"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I22" s="78"/>
-      <c r="J22" s="79"/>
+      <c r="I22" s="86"/>
+      <c r="J22" s="87"/>
     </row>
     <row r="23" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="83" t="s">
+      <c r="A23" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="84"/>
-      <c r="C23" s="84"/>
-      <c r="D23" s="84"/>
-      <c r="E23" s="84"/>
-      <c r="F23" s="84"/>
-      <c r="G23" s="84"/>
-      <c r="H23" s="84"/>
-      <c r="I23" s="84"/>
-      <c r="J23" s="85"/>
-      <c r="L23" s="31"/>
+      <c r="B23" s="92"/>
+      <c r="C23" s="92"/>
+      <c r="D23" s="92"/>
+      <c r="E23" s="92"/>
+      <c r="F23" s="92"/>
+      <c r="G23" s="92"/>
+      <c r="H23" s="92"/>
+      <c r="I23" s="92"/>
+      <c r="J23" s="93"/>
+      <c r="L23" s="26"/>
     </row>
     <row r="24" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="74"/>
-      <c r="C24" s="75"/>
-      <c r="D24" s="34" t="s">
+      <c r="B24" s="82"/>
+      <c r="C24" s="83"/>
+      <c r="D24" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="45"/>
-      <c r="F24" s="35" t="s">
+      <c r="E24" s="30"/>
+      <c r="F24" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="G24" s="23"/>
-      <c r="H24" s="48"/>
-      <c r="I24" s="30" t="s">
+      <c r="G24" s="21"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="J24" s="47"/>
+      <c r="J24" s="31"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="4"/>
       <c r="C25" s="5"/>
-      <c r="D25" s="17"/>
+      <c r="D25" s="15"/>
       <c r="E25" s="4"/>
-      <c r="F25" s="21"/>
+      <c r="F25" s="19"/>
       <c r="G25" s="10"/>
       <c r="H25" s="5"/>
-      <c r="I25" s="71" t="s">
+      <c r="I25" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="J25" s="64"/>
+      <c r="J25" s="72"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
       <c r="C26" s="5"/>
-      <c r="D26" s="69"/>
+      <c r="D26" s="77"/>
       <c r="E26" s="4"/>
-      <c r="F26" s="21"/>
+      <c r="F26" s="19"/>
       <c r="G26" s="10"/>
       <c r="H26" s="5"/>
-      <c r="I26" s="71"/>
-      <c r="J26" s="64"/>
+      <c r="I26" s="79"/>
+      <c r="J26" s="72"/>
     </row>
     <row r="27" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="4"/>
       <c r="C27" s="5"/>
-      <c r="D27" s="69"/>
+      <c r="D27" s="77"/>
       <c r="E27" s="4"/>
-      <c r="F27" s="21"/>
+      <c r="F27" s="19"/>
       <c r="G27" s="10"/>
       <c r="H27" s="5"/>
-      <c r="I27" s="72"/>
-      <c r="J27" s="65"/>
+      <c r="I27" s="80"/>
+      <c r="J27" s="73"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
@@ -1951,13 +1971,13 @@
       <c r="C28" s="5"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
-      <c r="F28" s="21"/>
+      <c r="F28" s="19"/>
       <c r="G28" s="10"/>
       <c r="H28" s="5"/>
-      <c r="I28" s="70" t="s">
+      <c r="I28" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="J28" s="64"/>
+      <c r="J28" s="72"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
@@ -1965,11 +1985,11 @@
       <c r="C29" s="5"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
-      <c r="F29" s="21"/>
+      <c r="F29" s="19"/>
       <c r="G29" s="10"/>
       <c r="H29" s="5"/>
-      <c r="I29" s="71"/>
-      <c r="J29" s="64"/>
+      <c r="I29" s="79"/>
+      <c r="J29" s="72"/>
     </row>
     <row r="30" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
@@ -1977,49 +1997,49 @@
       <c r="C30" s="5"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
-      <c r="F30" s="21"/>
+      <c r="F30" s="19"/>
       <c r="G30" s="10"/>
       <c r="H30" s="5"/>
-      <c r="I30" s="72"/>
-      <c r="J30" s="65"/>
+      <c r="I30" s="80"/>
+      <c r="J30" s="73"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="4"/>
       <c r="C31" s="5"/>
-      <c r="D31" s="17"/>
+      <c r="D31" s="15"/>
       <c r="E31" s="4"/>
-      <c r="F31" s="21"/>
+      <c r="F31" s="19"/>
       <c r="G31" s="10"/>
       <c r="H31" s="5"/>
-      <c r="I31" s="70" t="s">
+      <c r="I31" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="J31" s="64"/>
+      <c r="J31" s="72"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="4"/>
       <c r="C32" s="5"/>
-      <c r="D32" s="69"/>
+      <c r="D32" s="77"/>
       <c r="E32" s="4"/>
-      <c r="F32" s="21"/>
+      <c r="F32" s="19"/>
       <c r="G32" s="10"/>
       <c r="H32" s="5"/>
-      <c r="I32" s="71"/>
-      <c r="J32" s="64"/>
+      <c r="I32" s="79"/>
+      <c r="J32" s="72"/>
     </row>
     <row r="33" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
-      <c r="D33" s="69"/>
+      <c r="D33" s="77"/>
       <c r="E33" s="4"/>
-      <c r="F33" s="21"/>
+      <c r="F33" s="19"/>
       <c r="G33" s="10"/>
       <c r="H33" s="5"/>
-      <c r="I33" s="72"/>
-      <c r="J33" s="65"/>
+      <c r="I33" s="80"/>
+      <c r="J33" s="73"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
@@ -2027,13 +2047,13 @@
       <c r="C34" s="5"/>
       <c r="D34" s="3"/>
       <c r="E34" s="4"/>
-      <c r="F34" s="21"/>
+      <c r="F34" s="19"/>
       <c r="G34" s="10"/>
       <c r="H34" s="5"/>
-      <c r="I34" s="70" t="s">
+      <c r="I34" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="J34" s="64"/>
+      <c r="J34" s="72"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
@@ -2041,11 +2061,11 @@
       <c r="C35" s="5"/>
       <c r="D35" s="3"/>
       <c r="E35" s="4"/>
-      <c r="F35" s="21"/>
+      <c r="F35" s="19"/>
       <c r="G35" s="10"/>
       <c r="H35" s="5"/>
-      <c r="I35" s="71"/>
-      <c r="J35" s="64"/>
+      <c r="I35" s="79"/>
+      <c r="J35" s="72"/>
     </row>
     <row r="36" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
@@ -2053,11 +2073,11 @@
       <c r="C36" s="5"/>
       <c r="D36" s="3"/>
       <c r="E36" s="4"/>
-      <c r="F36" s="21"/>
+      <c r="F36" s="19"/>
       <c r="G36" s="10"/>
       <c r="H36" s="5"/>
-      <c r="I36" s="72"/>
-      <c r="J36" s="65"/>
+      <c r="I36" s="80"/>
+      <c r="J36" s="73"/>
     </row>
     <row r="37" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
@@ -2068,54 +2088,54 @@
       <c r="F37" s="3"/>
       <c r="G37" s="4"/>
       <c r="H37" s="5"/>
-      <c r="I37" s="70" t="s">
+      <c r="I37" s="78" t="s">
         <v>18</v>
       </c>
-      <c r="J37" s="64"/>
+      <c r="J37" s="72"/>
     </row>
     <row r="38" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="15"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="24" t="s">
+      <c r="A38" s="13"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E38" s="49"/>
-      <c r="F38" s="19"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="17"/>
       <c r="G38" s="10"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="71"/>
-      <c r="J38" s="64"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="79"/>
+      <c r="J38" s="72"/>
     </row>
     <row r="39" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="25" t="s">
+      <c r="A39" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="62"/>
-      <c r="C39" s="63"/>
-      <c r="D39" s="26" t="s">
+      <c r="B39" s="70"/>
+      <c r="C39" s="71"/>
+      <c r="D39" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="E39" s="50"/>
-      <c r="F39" s="15"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="20"/>
-      <c r="I39" s="72"/>
-      <c r="J39" s="65"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="80"/>
+      <c r="J39" s="73"/>
     </row>
     <row r="40" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="66" t="s">
+      <c r="A40" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="B40" s="67"/>
-      <c r="C40" s="67"/>
-      <c r="D40" s="67"/>
-      <c r="E40" s="67"/>
-      <c r="F40" s="67"/>
-      <c r="G40" s="67"/>
-      <c r="H40" s="67"/>
-      <c r="I40" s="67"/>
-      <c r="J40" s="68"/>
+      <c r="B40" s="75"/>
+      <c r="C40" s="75"/>
+      <c r="D40" s="75"/>
+      <c r="E40" s="75"/>
+      <c r="F40" s="75"/>
+      <c r="G40" s="75"/>
+      <c r="H40" s="75"/>
+      <c r="I40" s="75"/>
+      <c r="J40" s="76"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
@@ -2266,10 +2286,10 @@
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="2"/>
-      <c r="E53" s="70" t="s">
+      <c r="E53" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="F53" s="73"/>
+      <c r="F53" s="81"/>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
@@ -2280,8 +2300,8 @@
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="5"/>
-      <c r="E54" s="71"/>
-      <c r="F54" s="64"/>
+      <c r="E54" s="79"/>
+      <c r="F54" s="72"/>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
@@ -2292,8 +2312,8 @@
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="5"/>
-      <c r="E55" s="72"/>
-      <c r="F55" s="65"/>
+      <c r="E55" s="80"/>
+      <c r="F55" s="73"/>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
@@ -2304,10 +2324,10 @@
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="5"/>
-      <c r="E56" s="70" t="s">
+      <c r="E56" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="F56" s="73"/>
+      <c r="F56" s="81"/>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
@@ -2318,8 +2338,8 @@
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="5"/>
-      <c r="E57" s="71"/>
-      <c r="F57" s="64"/>
+      <c r="E57" s="79"/>
+      <c r="F57" s="72"/>
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
@@ -2330,8 +2350,8 @@
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="5"/>
-      <c r="E58" s="72"/>
-      <c r="F58" s="65"/>
+      <c r="E58" s="80"/>
+      <c r="F58" s="73"/>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
@@ -2342,10 +2362,10 @@
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="5"/>
-      <c r="E59" s="70" t="s">
+      <c r="E59" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="F59" s="73"/>
+      <c r="F59" s="81"/>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
@@ -2356,8 +2376,8 @@
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="5"/>
-      <c r="E60" s="71"/>
-      <c r="F60" s="64"/>
+      <c r="E60" s="79"/>
+      <c r="F60" s="72"/>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
@@ -2368,8 +2388,8 @@
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="5"/>
-      <c r="E61" s="72"/>
-      <c r="F61" s="65"/>
+      <c r="E61" s="80"/>
+      <c r="F61" s="73"/>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
@@ -2380,8 +2400,8 @@
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="5"/>
-      <c r="E62" s="52"/>
-      <c r="F62" s="51"/>
+      <c r="E62" s="36"/>
+      <c r="F62" s="35"/>
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
       <c r="I62" s="4"/>
@@ -2392,12 +2412,12 @@
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
       <c r="D63" s="8"/>
-      <c r="E63" s="53"/>
-      <c r="F63" s="54"/>
+      <c r="E63" s="37"/>
+      <c r="F63" s="38"/>
       <c r="G63" s="7"/>
       <c r="H63" s="7"/>
-      <c r="I63" s="60"/>
-      <c r="J63" s="61"/>
+      <c r="I63" s="68"/>
+      <c r="J63" s="69"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
@@ -2506,39 +2526,39 @@
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="55"/>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
+      <c r="A1" s="39"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="55"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
+      <c r="A2" s="39"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="55"/>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="55"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="55"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -2559,39 +2579,39 @@
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="55"/>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
+      <c r="A1" s="39"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="55"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
+      <c r="A2" s="39"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="55"/>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="55"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="55"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
end markların bulunması dbye kaydedilmesi
</commit_message>
<xml_diff>
--- a/WebApplication1/Forms/03_EgzozValf.xlsx
+++ b/WebApplication1/Forms/03_EgzozValf.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="4752" windowWidth="28560" windowHeight="10140"/>
+    <workbookView xWindow="120" yWindow="4752" windowWidth="28560" windowHeight="10140" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>VESSEL</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>{BuilderNo}</t>
+  </si>
+  <si>
+    <t>{END}</t>
   </si>
 </sst>
 </file>
@@ -563,19 +566,101 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -585,6 +670,39 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -593,124 +711,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1570,8 +1573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:J3"/>
+    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K57" sqref="K57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1582,42 +1585,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="91"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="71"/>
     </row>
     <row r="2" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="97" t="s">
+      <c r="B2" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="98"/>
-      <c r="D2" s="85" t="s">
+      <c r="C2" s="78"/>
+      <c r="D2" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="86"/>
-      <c r="F2" s="102" t="s">
+      <c r="E2" s="80"/>
+      <c r="F2" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="103"/>
+      <c r="G2" s="85"/>
       <c r="H2" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="95" t="s">
+      <c r="I2" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="96"/>
+      <c r="J2" s="76"/>
     </row>
     <row r="3" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="40" t="s">
@@ -1630,31 +1633,31 @@
         <v>35</v>
       </c>
       <c r="D3" s="66"/>
-      <c r="E3" s="104" t="s">
+      <c r="E3" s="86" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="105"/>
+      <c r="F3" s="87"/>
       <c r="G3" s="67"/>
       <c r="H3" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="97" t="s">
+      <c r="I3" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="98"/>
+      <c r="J3" s="78"/>
     </row>
     <row r="4" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="100"/>
-      <c r="C4" s="100"/>
-      <c r="D4" s="101"/>
+      <c r="B4" s="82"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="83"/>
       <c r="E4" s="68"/>
-      <c r="F4" s="85" t="s">
+      <c r="F4" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="86"/>
+      <c r="G4" s="80"/>
       <c r="H4" s="68"/>
       <c r="I4" s="40" t="s">
         <v>5</v>
@@ -1662,20 +1665,20 @@
       <c r="J4" s="68"/>
     </row>
     <row r="5" spans="1:16" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="109" t="s">
+      <c r="A5" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="110"/>
-      <c r="C5" s="110"/>
-      <c r="D5" s="111"/>
-      <c r="E5" s="106" t="s">
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="107"/>
-      <c r="G5" s="107"/>
-      <c r="H5" s="107"/>
-      <c r="I5" s="107"/>
-      <c r="J5" s="108"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="89"/>
+      <c r="H5" s="89"/>
+      <c r="I5" s="89"/>
+      <c r="J5" s="90"/>
       <c r="K5" s="29"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -1841,10 +1844,10 @@
       <c r="A19" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="112" t="s">
+      <c r="B19" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="113"/>
+      <c r="C19" s="95"/>
       <c r="D19" s="60" t="s">
         <v>31</v>
       </c>
@@ -1870,10 +1873,10 @@
       <c r="J20" s="54"/>
     </row>
     <row r="21" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="104" t="s">
+      <c r="A21" s="86" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="105"/>
+      <c r="B21" s="87"/>
       <c r="C21" s="63"/>
       <c r="D21" s="65" t="s">
         <v>33</v>
@@ -1886,44 +1889,44 @@
       <c r="J21" s="58"/>
     </row>
     <row r="22" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="104" t="s">
+      <c r="A22" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="105"/>
+      <c r="B22" s="87"/>
       <c r="C22" s="63"/>
       <c r="D22" s="64"/>
-      <c r="E22" s="85" t="s">
+      <c r="E22" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="86"/>
+      <c r="F22" s="80"/>
       <c r="G22" s="42"/>
       <c r="H22" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I22" s="87"/>
-      <c r="J22" s="88"/>
+      <c r="I22" s="103"/>
+      <c r="J22" s="104"/>
     </row>
     <row r="23" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="92" t="s">
+      <c r="A23" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="93"/>
-      <c r="C23" s="93"/>
-      <c r="D23" s="93"/>
-      <c r="E23" s="93"/>
-      <c r="F23" s="93"/>
-      <c r="G23" s="93"/>
-      <c r="H23" s="93"/>
-      <c r="I23" s="93"/>
-      <c r="J23" s="94"/>
+      <c r="B23" s="73"/>
+      <c r="C23" s="73"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="73"/>
+      <c r="F23" s="73"/>
+      <c r="G23" s="73"/>
+      <c r="H23" s="73"/>
+      <c r="I23" s="73"/>
+      <c r="J23" s="74"/>
       <c r="L23" s="26"/>
     </row>
     <row r="24" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="83"/>
-      <c r="C24" s="84"/>
+      <c r="B24" s="101"/>
+      <c r="C24" s="102"/>
       <c r="D24" s="27" t="s">
         <v>32</v>
       </c>
@@ -1947,34 +1950,34 @@
       <c r="F25" s="19"/>
       <c r="G25" s="10"/>
       <c r="H25" s="5"/>
-      <c r="I25" s="80" t="s">
+      <c r="I25" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="J25" s="73"/>
+      <c r="J25" s="99"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
       <c r="C26" s="5"/>
-      <c r="D26" s="78"/>
+      <c r="D26" s="105"/>
       <c r="E26" s="4"/>
       <c r="F26" s="19"/>
       <c r="G26" s="10"/>
       <c r="H26" s="5"/>
-      <c r="I26" s="80"/>
-      <c r="J26" s="73"/>
+      <c r="I26" s="97"/>
+      <c r="J26" s="99"/>
     </row>
     <row r="27" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="4"/>
       <c r="C27" s="5"/>
-      <c r="D27" s="78"/>
+      <c r="D27" s="105"/>
       <c r="E27" s="4"/>
       <c r="F27" s="19"/>
       <c r="G27" s="10"/>
       <c r="H27" s="5"/>
-      <c r="I27" s="81"/>
-      <c r="J27" s="74"/>
+      <c r="I27" s="98"/>
+      <c r="J27" s="100"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
@@ -1985,10 +1988,10 @@
       <c r="F28" s="19"/>
       <c r="G28" s="10"/>
       <c r="H28" s="5"/>
-      <c r="I28" s="79" t="s">
+      <c r="I28" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="J28" s="73"/>
+      <c r="J28" s="99"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
@@ -1999,8 +2002,8 @@
       <c r="F29" s="19"/>
       <c r="G29" s="10"/>
       <c r="H29" s="5"/>
-      <c r="I29" s="80"/>
-      <c r="J29" s="73"/>
+      <c r="I29" s="97"/>
+      <c r="J29" s="99"/>
     </row>
     <row r="30" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
@@ -2011,8 +2014,8 @@
       <c r="F30" s="19"/>
       <c r="G30" s="10"/>
       <c r="H30" s="5"/>
-      <c r="I30" s="81"/>
-      <c r="J30" s="74"/>
+      <c r="I30" s="98"/>
+      <c r="J30" s="100"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
@@ -2023,34 +2026,34 @@
       <c r="F31" s="19"/>
       <c r="G31" s="10"/>
       <c r="H31" s="5"/>
-      <c r="I31" s="79" t="s">
+      <c r="I31" s="96" t="s">
         <v>16</v>
       </c>
-      <c r="J31" s="73"/>
+      <c r="J31" s="99"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="4"/>
       <c r="C32" s="5"/>
-      <c r="D32" s="78"/>
+      <c r="D32" s="105"/>
       <c r="E32" s="4"/>
       <c r="F32" s="19"/>
       <c r="G32" s="10"/>
       <c r="H32" s="5"/>
-      <c r="I32" s="80"/>
-      <c r="J32" s="73"/>
+      <c r="I32" s="97"/>
+      <c r="J32" s="99"/>
     </row>
     <row r="33" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
-      <c r="D33" s="78"/>
+      <c r="D33" s="105"/>
       <c r="E33" s="4"/>
       <c r="F33" s="19"/>
       <c r="G33" s="10"/>
       <c r="H33" s="5"/>
-      <c r="I33" s="81"/>
-      <c r="J33" s="74"/>
+      <c r="I33" s="98"/>
+      <c r="J33" s="100"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
@@ -2061,10 +2064,10 @@
       <c r="F34" s="19"/>
       <c r="G34" s="10"/>
       <c r="H34" s="5"/>
-      <c r="I34" s="79" t="s">
+      <c r="I34" s="96" t="s">
         <v>17</v>
       </c>
-      <c r="J34" s="73"/>
+      <c r="J34" s="99"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
@@ -2075,8 +2078,8 @@
       <c r="F35" s="19"/>
       <c r="G35" s="10"/>
       <c r="H35" s="5"/>
-      <c r="I35" s="80"/>
-      <c r="J35" s="73"/>
+      <c r="I35" s="97"/>
+      <c r="J35" s="99"/>
     </row>
     <row r="36" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
@@ -2087,8 +2090,8 @@
       <c r="F36" s="19"/>
       <c r="G36" s="10"/>
       <c r="H36" s="5"/>
-      <c r="I36" s="81"/>
-      <c r="J36" s="74"/>
+      <c r="I36" s="98"/>
+      <c r="J36" s="100"/>
     </row>
     <row r="37" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
@@ -2099,10 +2102,10 @@
       <c r="F37" s="3"/>
       <c r="G37" s="4"/>
       <c r="H37" s="5"/>
-      <c r="I37" s="79" t="s">
+      <c r="I37" s="96" t="s">
         <v>18</v>
       </c>
-      <c r="J37" s="73"/>
+      <c r="J37" s="99"/>
     </row>
     <row r="38" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="13"/>
@@ -2115,15 +2118,15 @@
       <c r="F38" s="17"/>
       <c r="G38" s="10"/>
       <c r="H38" s="16"/>
-      <c r="I38" s="80"/>
-      <c r="J38" s="73"/>
+      <c r="I38" s="97"/>
+      <c r="J38" s="99"/>
     </row>
     <row r="39" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="71"/>
-      <c r="C39" s="72"/>
+      <c r="B39" s="108"/>
+      <c r="C39" s="109"/>
       <c r="D39" s="24" t="s">
         <v>24</v>
       </c>
@@ -2131,22 +2134,22 @@
       <c r="F39" s="13"/>
       <c r="G39" s="20"/>
       <c r="H39" s="18"/>
-      <c r="I39" s="81"/>
-      <c r="J39" s="74"/>
+      <c r="I39" s="98"/>
+      <c r="J39" s="100"/>
     </row>
     <row r="40" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="75" t="s">
+      <c r="A40" s="110" t="s">
         <v>19</v>
       </c>
-      <c r="B40" s="76"/>
-      <c r="C40" s="76"/>
-      <c r="D40" s="76"/>
-      <c r="E40" s="76"/>
-      <c r="F40" s="76"/>
-      <c r="G40" s="76"/>
-      <c r="H40" s="76"/>
-      <c r="I40" s="76"/>
-      <c r="J40" s="77"/>
+      <c r="B40" s="111"/>
+      <c r="C40" s="111"/>
+      <c r="D40" s="111"/>
+      <c r="E40" s="111"/>
+      <c r="F40" s="111"/>
+      <c r="G40" s="111"/>
+      <c r="H40" s="111"/>
+      <c r="I40" s="111"/>
+      <c r="J40" s="112"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
@@ -2297,10 +2300,10 @@
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="2"/>
-      <c r="E53" s="79" t="s">
+      <c r="E53" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="F53" s="82"/>
+      <c r="F53" s="113"/>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
@@ -2311,8 +2314,8 @@
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="5"/>
-      <c r="E54" s="80"/>
-      <c r="F54" s="73"/>
+      <c r="E54" s="97"/>
+      <c r="F54" s="99"/>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
@@ -2323,8 +2326,8 @@
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="5"/>
-      <c r="E55" s="81"/>
-      <c r="F55" s="74"/>
+      <c r="E55" s="98"/>
+      <c r="F55" s="100"/>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
@@ -2335,10 +2338,10 @@
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="5"/>
-      <c r="E56" s="79" t="s">
+      <c r="E56" s="96" t="s">
         <v>26</v>
       </c>
-      <c r="F56" s="82"/>
+      <c r="F56" s="113"/>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
@@ -2349,8 +2352,8 @@
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="5"/>
-      <c r="E57" s="80"/>
-      <c r="F57" s="73"/>
+      <c r="E57" s="97"/>
+      <c r="F57" s="99"/>
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
@@ -2361,8 +2364,8 @@
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="5"/>
-      <c r="E58" s="81"/>
-      <c r="F58" s="74"/>
+      <c r="E58" s="98"/>
+      <c r="F58" s="100"/>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
@@ -2373,10 +2376,10 @@
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="5"/>
-      <c r="E59" s="79" t="s">
+      <c r="E59" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="F59" s="82"/>
+      <c r="F59" s="113"/>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
@@ -2387,8 +2390,8 @@
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="5"/>
-      <c r="E60" s="80"/>
-      <c r="F60" s="73"/>
+      <c r="E60" s="97"/>
+      <c r="F60" s="99"/>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
@@ -2399,8 +2402,8 @@
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="5"/>
-      <c r="E61" s="81"/>
-      <c r="F61" s="74"/>
+      <c r="E61" s="98"/>
+      <c r="F61" s="100"/>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
@@ -2427,8 +2430,8 @@
       <c r="F63" s="38"/>
       <c r="G63" s="7"/>
       <c r="H63" s="7"/>
-      <c r="I63" s="69"/>
-      <c r="J63" s="70"/>
+      <c r="I63" s="106"/>
+      <c r="J63" s="107"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
@@ -2441,7 +2444,9 @@
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
       <c r="J64" s="4"/>
-      <c r="K64" s="4"/>
+      <c r="K64" s="4" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
@@ -2477,6 +2482,30 @@
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <dataConsolidate/>
   <mergeCells count="39">
+    <mergeCell ref="I63:J63"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="J37:J39"/>
+    <mergeCell ref="A40:J40"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="I37:I39"/>
+    <mergeCell ref="E53:E55"/>
+    <mergeCell ref="E56:E58"/>
+    <mergeCell ref="E59:E61"/>
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="F56:F58"/>
+    <mergeCell ref="F59:F61"/>
+    <mergeCell ref="J34:J36"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="I25:I27"/>
+    <mergeCell ref="I28:I30"/>
+    <mergeCell ref="J25:J27"/>
+    <mergeCell ref="I31:I33"/>
+    <mergeCell ref="I34:I36"/>
+    <mergeCell ref="J28:J30"/>
+    <mergeCell ref="J31:J33"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A23:J23"/>
     <mergeCell ref="I2:J2"/>
@@ -2492,30 +2521,6 @@
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="A22:B22"/>
-    <mergeCell ref="I28:I30"/>
-    <mergeCell ref="J25:J27"/>
-    <mergeCell ref="I31:I33"/>
-    <mergeCell ref="I34:I36"/>
-    <mergeCell ref="J28:J30"/>
-    <mergeCell ref="J31:J33"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="I25:I27"/>
-    <mergeCell ref="I63:J63"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="J37:J39"/>
-    <mergeCell ref="A40:J40"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="I37:I39"/>
-    <mergeCell ref="E53:E55"/>
-    <mergeCell ref="E56:E58"/>
-    <mergeCell ref="E59:E61"/>
-    <mergeCell ref="F53:F55"/>
-    <mergeCell ref="F56:F58"/>
-    <mergeCell ref="F59:F61"/>
-    <mergeCell ref="J34:J36"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2528,48 +2533,53 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="39"/>
       <c r="B1" s="39"/>
       <c r="C1" s="39"/>
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="39"/>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="39"/>
       <c r="B3" s="39"/>
       <c r="C3" s="39"/>
       <c r="D3" s="39"/>
       <c r="E3" s="39"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="39"/>
       <c r="B4" s="39"/>
       <c r="C4" s="39"/>
       <c r="D4" s="39"/>
       <c r="E4" s="39"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="39"/>
       <c r="B5" s="39"/>
       <c r="C5" s="39"/>
       <c r="D5" s="39"/>
       <c r="E5" s="39"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -2581,48 +2591,53 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="39"/>
       <c r="B1" s="39"/>
       <c r="C1" s="39"/>
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="39"/>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="39"/>
       <c r="B3" s="39"/>
       <c r="C3" s="39"/>
       <c r="D3" s="39"/>
       <c r="E3" s="39"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="39"/>
       <c r="B4" s="39"/>
       <c r="C4" s="39"/>
       <c r="D4" s="39"/>
       <c r="E4" s="39"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="39"/>
       <c r="B5" s="39"/>
       <c r="C5" s="39"/>
       <c r="D5" s="39"/>
       <c r="E5" s="39"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
defaultarın liste olarak gosterilmesi
</commit_message>
<xml_diff>
--- a/WebApplication1/Forms/03_EgzozValf.xlsx
+++ b/WebApplication1/Forms/03_EgzozValf.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
   <si>
     <t>VESSEL</t>
   </si>
@@ -134,9 +134,6 @@
     <t>De-Mounted fr Cyl.</t>
   </si>
   <si>
-    <t>{VesselName}</t>
-  </si>
-  <si>
     <t>{BuilderNo}</t>
   </si>
   <si>
@@ -144,6 +141,15 @@
   </si>
   <si>
     <t>{E}</t>
+  </si>
+  <si>
+    <t>bir</t>
+  </si>
+  <si>
+    <t>iki</t>
+  </si>
+  <si>
+    <t>{testDefault}</t>
   </si>
 </sst>
 </file>
@@ -566,19 +572,101 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -588,6 +676,39 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -596,124 +717,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1574,7 +1580,7 @@
   <dimension ref="A1:P76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:C19"/>
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1585,40 +1591,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="91"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="71"/>
+      <c r="K1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="2" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="98"/>
-      <c r="D2" s="85" t="s">
+      <c r="B2" s="77" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="78"/>
+      <c r="D2" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="86"/>
-      <c r="F2" s="102" t="s">
+      <c r="E2" s="80"/>
+      <c r="F2" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="103"/>
+      <c r="G2" s="85"/>
       <c r="H2" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="95"/>
-      <c r="J2" s="96"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="76"/>
+      <c r="K2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="3" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="40" t="s">
@@ -1629,31 +1641,31 @@
         <v>35</v>
       </c>
       <c r="D3" s="66"/>
-      <c r="E3" s="104" t="s">
+      <c r="E3" s="86" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="105"/>
+      <c r="F3" s="87"/>
       <c r="G3" s="67"/>
       <c r="H3" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="97" t="s">
-        <v>38</v>
-      </c>
-      <c r="J3" s="98"/>
+      <c r="I3" s="77" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="78"/>
     </row>
     <row r="4" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="100"/>
-      <c r="C4" s="100"/>
-      <c r="D4" s="101"/>
+      <c r="B4" s="82"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="83"/>
       <c r="E4" s="68"/>
-      <c r="F4" s="85" t="s">
+      <c r="F4" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="86"/>
+      <c r="G4" s="80"/>
       <c r="H4" s="68"/>
       <c r="I4" s="40" t="s">
         <v>5</v>
@@ -1661,20 +1673,20 @@
       <c r="J4" s="68"/>
     </row>
     <row r="5" spans="1:16" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="109" t="s">
+      <c r="A5" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="110"/>
-      <c r="C5" s="110"/>
-      <c r="D5" s="111"/>
-      <c r="E5" s="106" t="s">
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="107"/>
-      <c r="G5" s="107"/>
-      <c r="H5" s="107"/>
-      <c r="I5" s="107"/>
-      <c r="J5" s="108"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="89"/>
+      <c r="H5" s="89"/>
+      <c r="I5" s="89"/>
+      <c r="J5" s="90"/>
       <c r="K5" s="29"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -1840,8 +1852,8 @@
       <c r="A19" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="112"/>
-      <c r="C19" s="113"/>
+      <c r="B19" s="94"/>
+      <c r="C19" s="95"/>
       <c r="D19" s="60" t="s">
         <v>31</v>
       </c>
@@ -1867,10 +1879,10 @@
       <c r="J20" s="54"/>
     </row>
     <row r="21" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="104" t="s">
+      <c r="A21" s="86" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="105"/>
+      <c r="B21" s="87"/>
       <c r="C21" s="63"/>
       <c r="D21" s="65" t="s">
         <v>33</v>
@@ -1883,44 +1895,44 @@
       <c r="J21" s="58"/>
     </row>
     <row r="22" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="104" t="s">
+      <c r="A22" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="105"/>
+      <c r="B22" s="87"/>
       <c r="C22" s="63"/>
       <c r="D22" s="64"/>
-      <c r="E22" s="85" t="s">
+      <c r="E22" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="86"/>
+      <c r="F22" s="80"/>
       <c r="G22" s="42"/>
       <c r="H22" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I22" s="87"/>
-      <c r="J22" s="88"/>
+      <c r="I22" s="103"/>
+      <c r="J22" s="104"/>
     </row>
     <row r="23" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="92" t="s">
+      <c r="A23" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="93"/>
-      <c r="C23" s="93"/>
-      <c r="D23" s="93"/>
-      <c r="E23" s="93"/>
-      <c r="F23" s="93"/>
-      <c r="G23" s="93"/>
-      <c r="H23" s="93"/>
-      <c r="I23" s="93"/>
-      <c r="J23" s="94"/>
+      <c r="B23" s="73"/>
+      <c r="C23" s="73"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="73"/>
+      <c r="F23" s="73"/>
+      <c r="G23" s="73"/>
+      <c r="H23" s="73"/>
+      <c r="I23" s="73"/>
+      <c r="J23" s="74"/>
       <c r="L23" s="26"/>
     </row>
     <row r="24" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="83"/>
-      <c r="C24" s="84"/>
+      <c r="B24" s="101"/>
+      <c r="C24" s="102"/>
       <c r="D24" s="27" t="s">
         <v>32</v>
       </c>
@@ -1944,34 +1956,34 @@
       <c r="F25" s="19"/>
       <c r="G25" s="10"/>
       <c r="H25" s="5"/>
-      <c r="I25" s="80" t="s">
+      <c r="I25" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="J25" s="73"/>
+      <c r="J25" s="99"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
       <c r="C26" s="5"/>
-      <c r="D26" s="78"/>
+      <c r="D26" s="105"/>
       <c r="E26" s="4"/>
       <c r="F26" s="19"/>
       <c r="G26" s="10"/>
       <c r="H26" s="5"/>
-      <c r="I26" s="80"/>
-      <c r="J26" s="73"/>
+      <c r="I26" s="97"/>
+      <c r="J26" s="99"/>
     </row>
     <row r="27" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="4"/>
       <c r="C27" s="5"/>
-      <c r="D27" s="78"/>
+      <c r="D27" s="105"/>
       <c r="E27" s="4"/>
       <c r="F27" s="19"/>
       <c r="G27" s="10"/>
       <c r="H27" s="5"/>
-      <c r="I27" s="81"/>
-      <c r="J27" s="74"/>
+      <c r="I27" s="98"/>
+      <c r="J27" s="100"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
@@ -1982,10 +1994,10 @@
       <c r="F28" s="19"/>
       <c r="G28" s="10"/>
       <c r="H28" s="5"/>
-      <c r="I28" s="79" t="s">
+      <c r="I28" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="J28" s="73"/>
+      <c r="J28" s="99"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
@@ -1996,8 +2008,8 @@
       <c r="F29" s="19"/>
       <c r="G29" s="10"/>
       <c r="H29" s="5"/>
-      <c r="I29" s="80"/>
-      <c r="J29" s="73"/>
+      <c r="I29" s="97"/>
+      <c r="J29" s="99"/>
     </row>
     <row r="30" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
@@ -2008,8 +2020,8 @@
       <c r="F30" s="19"/>
       <c r="G30" s="10"/>
       <c r="H30" s="5"/>
-      <c r="I30" s="81"/>
-      <c r="J30" s="74"/>
+      <c r="I30" s="98"/>
+      <c r="J30" s="100"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
@@ -2020,34 +2032,34 @@
       <c r="F31" s="19"/>
       <c r="G31" s="10"/>
       <c r="H31" s="5"/>
-      <c r="I31" s="79" t="s">
+      <c r="I31" s="96" t="s">
         <v>16</v>
       </c>
-      <c r="J31" s="73"/>
+      <c r="J31" s="99"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="4"/>
       <c r="C32" s="5"/>
-      <c r="D32" s="78"/>
+      <c r="D32" s="105"/>
       <c r="E32" s="4"/>
       <c r="F32" s="19"/>
       <c r="G32" s="10"/>
       <c r="H32" s="5"/>
-      <c r="I32" s="80"/>
-      <c r="J32" s="73"/>
+      <c r="I32" s="97"/>
+      <c r="J32" s="99"/>
     </row>
     <row r="33" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
-      <c r="D33" s="78"/>
+      <c r="D33" s="105"/>
       <c r="E33" s="4"/>
       <c r="F33" s="19"/>
       <c r="G33" s="10"/>
       <c r="H33" s="5"/>
-      <c r="I33" s="81"/>
-      <c r="J33" s="74"/>
+      <c r="I33" s="98"/>
+      <c r="J33" s="100"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
@@ -2058,10 +2070,10 @@
       <c r="F34" s="19"/>
       <c r="G34" s="10"/>
       <c r="H34" s="5"/>
-      <c r="I34" s="79" t="s">
+      <c r="I34" s="96" t="s">
         <v>17</v>
       </c>
-      <c r="J34" s="73"/>
+      <c r="J34" s="99"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
@@ -2072,8 +2084,8 @@
       <c r="F35" s="19"/>
       <c r="G35" s="10"/>
       <c r="H35" s="5"/>
-      <c r="I35" s="80"/>
-      <c r="J35" s="73"/>
+      <c r="I35" s="97"/>
+      <c r="J35" s="99"/>
     </row>
     <row r="36" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
@@ -2084,8 +2096,8 @@
       <c r="F36" s="19"/>
       <c r="G36" s="10"/>
       <c r="H36" s="5"/>
-      <c r="I36" s="81"/>
-      <c r="J36" s="74"/>
+      <c r="I36" s="98"/>
+      <c r="J36" s="100"/>
     </row>
     <row r="37" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
@@ -2096,10 +2108,10 @@
       <c r="F37" s="3"/>
       <c r="G37" s="4"/>
       <c r="H37" s="5"/>
-      <c r="I37" s="79" t="s">
+      <c r="I37" s="96" t="s">
         <v>18</v>
       </c>
-      <c r="J37" s="73"/>
+      <c r="J37" s="99"/>
     </row>
     <row r="38" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="13"/>
@@ -2112,15 +2124,15 @@
       <c r="F38" s="17"/>
       <c r="G38" s="10"/>
       <c r="H38" s="16"/>
-      <c r="I38" s="80"/>
-      <c r="J38" s="73"/>
+      <c r="I38" s="97"/>
+      <c r="J38" s="99"/>
     </row>
     <row r="39" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="71"/>
-      <c r="C39" s="72"/>
+      <c r="B39" s="108"/>
+      <c r="C39" s="109"/>
       <c r="D39" s="24" t="s">
         <v>24</v>
       </c>
@@ -2128,22 +2140,22 @@
       <c r="F39" s="13"/>
       <c r="G39" s="20"/>
       <c r="H39" s="18"/>
-      <c r="I39" s="81"/>
-      <c r="J39" s="74"/>
+      <c r="I39" s="98"/>
+      <c r="J39" s="100"/>
     </row>
     <row r="40" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="75" t="s">
+      <c r="A40" s="110" t="s">
         <v>19</v>
       </c>
-      <c r="B40" s="76"/>
-      <c r="C40" s="76"/>
-      <c r="D40" s="76"/>
-      <c r="E40" s="76"/>
-      <c r="F40" s="76"/>
-      <c r="G40" s="76"/>
-      <c r="H40" s="76"/>
-      <c r="I40" s="76"/>
-      <c r="J40" s="77"/>
+      <c r="B40" s="111"/>
+      <c r="C40" s="111"/>
+      <c r="D40" s="111"/>
+      <c r="E40" s="111"/>
+      <c r="F40" s="111"/>
+      <c r="G40" s="111"/>
+      <c r="H40" s="111"/>
+      <c r="I40" s="111"/>
+      <c r="J40" s="112"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
@@ -2294,10 +2306,10 @@
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="2"/>
-      <c r="E53" s="79" t="s">
+      <c r="E53" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="F53" s="82"/>
+      <c r="F53" s="113"/>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
@@ -2308,8 +2320,8 @@
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="5"/>
-      <c r="E54" s="80"/>
-      <c r="F54" s="73"/>
+      <c r="E54" s="97"/>
+      <c r="F54" s="99"/>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
@@ -2320,8 +2332,8 @@
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="5"/>
-      <c r="E55" s="81"/>
-      <c r="F55" s="74"/>
+      <c r="E55" s="98"/>
+      <c r="F55" s="100"/>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
@@ -2332,10 +2344,10 @@
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="5"/>
-      <c r="E56" s="79" t="s">
+      <c r="E56" s="96" t="s">
         <v>26</v>
       </c>
-      <c r="F56" s="82"/>
+      <c r="F56" s="113"/>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
@@ -2346,8 +2358,8 @@
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="5"/>
-      <c r="E57" s="80"/>
-      <c r="F57" s="73"/>
+      <c r="E57" s="97"/>
+      <c r="F57" s="99"/>
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
@@ -2358,8 +2370,8 @@
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="5"/>
-      <c r="E58" s="81"/>
-      <c r="F58" s="74"/>
+      <c r="E58" s="98"/>
+      <c r="F58" s="100"/>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
@@ -2370,10 +2382,10 @@
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="5"/>
-      <c r="E59" s="79" t="s">
+      <c r="E59" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="F59" s="82"/>
+      <c r="F59" s="113"/>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
@@ -2384,8 +2396,8 @@
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="5"/>
-      <c r="E60" s="80"/>
-      <c r="F60" s="73"/>
+      <c r="E60" s="97"/>
+      <c r="F60" s="99"/>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
@@ -2396,8 +2408,8 @@
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="5"/>
-      <c r="E61" s="81"/>
-      <c r="F61" s="74"/>
+      <c r="E61" s="98"/>
+      <c r="F61" s="100"/>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
@@ -2424,8 +2436,8 @@
       <c r="F63" s="38"/>
       <c r="G63" s="7"/>
       <c r="H63" s="7"/>
-      <c r="I63" s="69"/>
-      <c r="J63" s="70"/>
+      <c r="I63" s="106"/>
+      <c r="J63" s="107"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
@@ -2439,7 +2451,7 @@
       <c r="I64" s="4"/>
       <c r="J64" s="4"/>
       <c r="K64" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
@@ -2476,6 +2488,30 @@
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <dataConsolidate/>
   <mergeCells count="39">
+    <mergeCell ref="I63:J63"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="J37:J39"/>
+    <mergeCell ref="A40:J40"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="I37:I39"/>
+    <mergeCell ref="E53:E55"/>
+    <mergeCell ref="E56:E58"/>
+    <mergeCell ref="E59:E61"/>
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="F56:F58"/>
+    <mergeCell ref="F59:F61"/>
+    <mergeCell ref="J34:J36"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="I25:I27"/>
+    <mergeCell ref="I28:I30"/>
+    <mergeCell ref="J25:J27"/>
+    <mergeCell ref="I31:I33"/>
+    <mergeCell ref="I34:I36"/>
+    <mergeCell ref="J28:J30"/>
+    <mergeCell ref="J31:J33"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A23:J23"/>
     <mergeCell ref="I2:J2"/>
@@ -2491,30 +2527,6 @@
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="A22:B22"/>
-    <mergeCell ref="I28:I30"/>
-    <mergeCell ref="J25:J27"/>
-    <mergeCell ref="I31:I33"/>
-    <mergeCell ref="I34:I36"/>
-    <mergeCell ref="J28:J30"/>
-    <mergeCell ref="J31:J33"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="I25:I27"/>
-    <mergeCell ref="I63:J63"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="J37:J39"/>
-    <mergeCell ref="A40:J40"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="I37:I39"/>
-    <mergeCell ref="E53:E55"/>
-    <mergeCell ref="E56:E58"/>
-    <mergeCell ref="E59:E61"/>
-    <mergeCell ref="F53:F55"/>
-    <mergeCell ref="F56:F58"/>
-    <mergeCell ref="F59:F61"/>
-    <mergeCell ref="J34:J36"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2572,7 +2584,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2630,7 +2642,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>